<commit_message>
Fixed ENV_ACT for FerroAlloys
Was FLO_EMIS, which we dont/cant use anymore
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-FA.xlsx
+++ b/vt_REGION1_IND-FA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD4066E-411B-445E-8166-F1DAAFA43B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ECA1A3-94FA-4B7D-8804-7B93CA52888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7530" yWindow="6900" windowWidth="23625" windowHeight="12240" tabRatio="842" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About and Log" sheetId="64" r:id="rId1"/>
@@ -24309,7 +24309,7 @@
   <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26511,10 +26511,10 @@
   <sheetPr>
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="M26:N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26785,9 +26785,6 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="313"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -26804,11 +26801,11 @@
   </sheetPr>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="6" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -27017,16 +27014,16 @@
         <v>193</v>
       </c>
       <c r="O7" s="92" t="str">
-        <f>"FLO_EMIS~"&amp;O5</f>
-        <v>FLO_EMIS~CO2SPIFC</v>
+        <f>"ENV_ACT~"&amp;O5</f>
+        <v>ENV_ACT~CO2SPIFC</v>
       </c>
       <c r="P7" s="92" t="str">
-        <f>"FLO_EMIS~"&amp;P5</f>
-        <v>FLO_EMIS~CO2SPIFM</v>
+        <f>"ENV_ACT~"&amp;P5</f>
+        <v>ENV_ACT~CO2SPIFM</v>
       </c>
       <c r="Q7" s="92" t="str">
-        <f>"FLO_EMIS~"&amp;Q5</f>
-        <v>FLO_EMIS~CH4S</v>
+        <f>"ENV_ACT~"&amp;Q5</f>
+        <v>ENV_ACT~CH4S</v>
       </c>
       <c r="R7" s="31" t="s">
         <v>145</v>

</xml_diff>

<commit_message>
Added missing bits to metals industry
numerous small tweaks for debugging.

added coke ovens so we have coke for I&S and FA. note it's in I&S sheet.
added transfer tech for INDCOA to IISCOA. will need to consider how the emissions will be accounted.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-FA.xlsx
+++ b/vt_REGION1_IND-FA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4ECA1A3-94FA-4B7D-8804-7B93CA52888B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5BDD57-F4B5-429C-90E3-DF8BA47BDF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="842" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="842" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About and Log" sheetId="64" r:id="rId1"/>
@@ -43,13 +43,9 @@
     <sheet name="ANSv2-692-TID TRADE" sheetId="16" state="veryHidden" r:id="rId28"/>
     <sheet name="ANSv2-692-TS&amp;TID TRADE" sheetId="17" state="veryHidden" r:id="rId29"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId30"/>
-    <externalReference r:id="rId31"/>
-  </externalReferences>
   <definedNames>
     <definedName name="FA_PAMS_index">Index!$J$5</definedName>
-    <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
+    <definedName name="FID_1">#REF!</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="7" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="17" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="6" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -939,30 +935,8 @@
 </comments>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="601">
   <si>
     <t>Comment</t>
   </si>
@@ -3073,6 +3047,30 @@
   </si>
   <si>
     <t>*TechDesc</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>*Unit</t>
+  </si>
+  <si>
+    <t>Demand Commodity Name</t>
+  </si>
+  <si>
+    <t>Demand Unit</t>
+  </si>
+  <si>
+    <t>Demand Value</t>
+  </si>
+  <si>
+    <t>Demand</t>
+  </si>
+  <si>
+    <t>PRC_CAPACT</t>
+  </si>
+  <si>
+    <t>ACT_BND~LO~2017</t>
   </si>
 </sst>
 </file>
@@ -4397,7 +4395,7 @@
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="332">
+  <cellXfs count="333">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4995,6 +4993,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="33" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -19664,335 +19663,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="IEA Data"/>
-      <sheetName val="E&amp;D Drivers"/>
-      <sheetName val="AGR_Fuels"/>
-      <sheetName val="AGR"/>
-      <sheetName val="RES_Fuels"/>
-      <sheetName val="RH1"/>
-      <sheetName val="RH2"/>
-      <sheetName val="RH3"/>
-      <sheetName val="RH4"/>
-      <sheetName val="RC1"/>
-      <sheetName val="RC2"/>
-      <sheetName val="RC3"/>
-      <sheetName val="RC4"/>
-      <sheetName val="RHW"/>
-      <sheetName val="RRF"/>
-      <sheetName val="RCW"/>
-      <sheetName val="RCD"/>
-      <sheetName val="RK1"/>
-      <sheetName val="RK2"/>
-      <sheetName val="RK3"/>
-      <sheetName val="RK4"/>
-      <sheetName val="RDW"/>
-      <sheetName val="RME"/>
-      <sheetName val="RL1"/>
-      <sheetName val="RL2"/>
-      <sheetName val="RL3"/>
-      <sheetName val="RL4"/>
-      <sheetName val="COM_Fuels"/>
-      <sheetName val="CH1"/>
-      <sheetName val="CH2"/>
-      <sheetName val="CH3"/>
-      <sheetName val="CH4"/>
-      <sheetName val="CC1"/>
-      <sheetName val="CC2"/>
-      <sheetName val="CC3"/>
-      <sheetName val="CC4"/>
-      <sheetName val="CHW"/>
-      <sheetName val="CAA"/>
-      <sheetName val="CLA"/>
-      <sheetName val="ElastPar"/>
-      <sheetName val="Conversion Factors"/>
-      <sheetName val="Intro"/>
-      <sheetName val="TechRep"/>
-      <sheetName val="Other_HYDRO"/>
-      <sheetName val="Other_NUCL"/>
-      <sheetName val="Other_THERM"/>
-      <sheetName val="Other_CHP"/>
-      <sheetName val="Other_RENEW"/>
-      <sheetName val="Other_HEAT"/>
-      <sheetName val="ELC_FUELS"/>
-      <sheetName val="ELC"/>
-      <sheetName val="HEAT"/>
-      <sheetName val="CHP"/>
-      <sheetName val="ELC_EMI"/>
-      <sheetName val="Constant Table"/>
-      <sheetName val="ANS_ITEMS_DEL"/>
-      <sheetName val="ANS_ITEMS"/>
-      <sheetName val="ANS_TIDDATA"/>
-      <sheetName val="ANS_TSDATA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>^FI_ST: TCH, PRC</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Index"/>
-      <sheetName val="ChangeLog"/>
-      <sheetName val="NameConv"/>
-      <sheetName val="Industry desription"/>
-      <sheetName val="SIC codes"/>
-      <sheetName val="REGIONS"/>
-      <sheetName val="Detailed GDP STATSSA"/>
-      <sheetName val="GDP STATSSA"/>
-      <sheetName val="Output compiled"/>
-      <sheetName val="IND GDP statssa 2"/>
-      <sheetName val="Ind output Mark"/>
-      <sheetName val="Ind mining output STATSSA"/>
-      <sheetName val="Ind Man output STATSSA"/>
-      <sheetName val="supply and use tables"/>
-      <sheetName val="DOE 2006 native units"/>
-      <sheetName val="2006-2009"/>
-      <sheetName val="Industry VA"/>
-      <sheetName val="Sources"/>
-      <sheetName val="1992-2006 industry"/>
-      <sheetName val="DoE2013 Industry EB"/>
-      <sheetName val="digest "/>
-      <sheetName val="DMR1"/>
-      <sheetName val="mining general info"/>
-      <sheetName val="I&amp;S - prod"/>
-      <sheetName val="I&amp;S - prod 2"/>
-      <sheetName val="I&amp;S - prod 3"/>
-      <sheetName val="End uses"/>
-      <sheetName val="EIA end use"/>
-      <sheetName val="Aluminium"/>
-      <sheetName val="Eskom sales data"/>
-      <sheetName val="Eskom Annual YB"/>
-      <sheetName val="eskom yb sector sales"/>
-      <sheetName val="NERSA Elec"/>
-      <sheetName val="REPORT TABLES"/>
-      <sheetName val="Tech Efficiencies"/>
-      <sheetName val="Coal prices"/>
-      <sheetName val="Electricity prices"/>
-      <sheetName val="ELEC CALCS ADRIAN IGNORE"/>
-      <sheetName val="FA-Items"/>
-      <sheetName val="FA-TSData"/>
-      <sheetName val="FA-TIDData"/>
-      <sheetName val="FerroAlloys"/>
-      <sheetName val="Aluminium - Items"/>
-      <sheetName val="Aluminium - TIDData"/>
-      <sheetName val="Aluminium - TSData"/>
-      <sheetName val="Aluminium Data"/>
-      <sheetName val="NMM-Items"/>
-      <sheetName val="NMM-TSData"/>
-      <sheetName val="NMM-TIDData"/>
-      <sheetName val="NMM data"/>
-      <sheetName val="Coking coal"/>
-      <sheetName val="COGEN"/>
-      <sheetName val="Payback from EIA"/>
-      <sheetName val="SasolGasSales"/>
-      <sheetName val="2012 SATIM EB"/>
-      <sheetName val="2017 SATIM EB"/>
-      <sheetName val="IND old - 2006BY"/>
-      <sheetName val="IND"/>
-      <sheetName val="IND2017"/>
-      <sheetName val="PAMS central control panel"/>
-      <sheetName val="ITEMS_Tech"/>
-      <sheetName val="ITEMS_Comm"/>
-      <sheetName val="TS DTech"/>
-      <sheetName val="TS DMARK"/>
-      <sheetName val="TID DTech"/>
-      <sheetName val="TS BYDem"/>
-      <sheetName val="TS COMFRN"/>
-      <sheetName val="TS COMFR"/>
-      <sheetName val="TS COMFRN_10"/>
-      <sheetName val="TS COMFR_10"/>
-      <sheetName val="TS ETech"/>
-      <sheetName val="TID ETech"/>
-      <sheetName val="TS GTech"/>
-      <sheetName val="TID GTech"/>
-      <sheetName val="TS FTech"/>
-      <sheetName val="TID FTech"/>
-      <sheetName val="TS Emiss"/>
-      <sheetName val="TID Emiss"/>
-      <sheetName val="AFA"/>
-      <sheetName val="Sc1 Standards"/>
-      <sheetName val="Sc2 Audits"/>
-      <sheetName val="Sc3 En Man"/>
-      <sheetName val="Sc4 Accreditation"/>
-      <sheetName val="Sc5 Education"/>
-      <sheetName val="Sc6 NEEA"/>
-      <sheetName val="Sc7 Finance"/>
-      <sheetName val="TCH_IND"/>
-    </sheetNames>
-    <definedNames>
-      <definedName name="pamsindex" refersTo="='PAMS central control panel'!$C$2"/>
-    </definedNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59">
-        <row r="2">
-          <cell r="C2" t="b">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-      <sheetData sheetId="86" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20921,13 +20591,13 @@
   <sheetPr codeName="Sheet17">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E25"/>
+      <selection pane="bottomRight" activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -21015,6 +20685,71 @@
     <row r="10" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C19" s="3" t="str">
+        <f>B8</f>
+        <v>IFAMN</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="317">
+        <f>E8</f>
+        <v>0.4587</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>598</v>
+      </c>
+      <c r="C20" s="3" t="str">
+        <f>B9</f>
+        <v>IFACR</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="317">
+        <f>E9</f>
+        <v>3.484</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="0" r:id="rId1"/>
@@ -21632,7 +21367,7 @@
         <v>IFACR</v>
       </c>
       <c r="H9" s="131">
-        <f>'Process Input'!T11</f>
+        <f>'Process Input'!U11</f>
         <v>12.360988518943744</v>
       </c>
       <c r="I9" s="94">
@@ -21738,7 +21473,7 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="323" t="s">
+      <c r="B3" s="324" t="s">
         <v>241</v>
       </c>
       <c r="C3" s="140" t="s">
@@ -21747,14 +21482,14 @@
       <c r="E3" s="141"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="323"/>
+      <c r="B4" s="324"/>
       <c r="C4" s="140" t="s">
         <v>243</v>
       </c>
       <c r="E4" s="141"/>
     </row>
     <row r="5" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="324"/>
+      <c r="B5" s="325"/>
       <c r="C5" s="142" t="s">
         <v>244</v>
       </c>
@@ -21764,7 +21499,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="325" t="s">
+      <c r="B6" s="326" t="s">
         <v>246</v>
       </c>
       <c r="C6" s="143" t="s">
@@ -21776,7 +21511,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="326"/>
+      <c r="B7" s="327"/>
       <c r="C7" s="143" t="s">
         <v>249</v>
       </c>
@@ -21786,14 +21521,14 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="327"/>
+      <c r="B8" s="328"/>
       <c r="C8" s="144" t="s">
         <v>250</v>
       </c>
       <c r="E8" s="141"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="325" t="s">
+      <c r="B9" s="326" t="s">
         <v>251</v>
       </c>
       <c r="C9" s="143" t="s">
@@ -21805,7 +21540,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="326"/>
+      <c r="B10" s="327"/>
       <c r="C10" s="143" t="s">
         <v>253</v>
       </c>
@@ -21815,7 +21550,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="327"/>
+      <c r="B11" s="328"/>
       <c r="C11" s="144" t="s">
         <v>255</v>
       </c>
@@ -21825,7 +21560,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="325" t="s">
+      <c r="B12" s="326" t="s">
         <v>257</v>
       </c>
       <c r="C12" s="143" t="s">
@@ -21834,14 +21569,14 @@
       <c r="E12" s="141"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="326"/>
+      <c r="B13" s="327"/>
       <c r="C13" s="143" t="s">
         <v>253</v>
       </c>
       <c r="E13" s="141"/>
     </row>
     <row r="14" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="327"/>
+      <c r="B14" s="328"/>
       <c r="C14" s="144" t="s">
         <v>258</v>
       </c>
@@ -21951,10 +21686,10 @@
       <c r="B21" s="150" t="s">
         <v>273</v>
       </c>
-      <c r="C21" s="321">
+      <c r="C21" s="322">
         <v>1200</v>
       </c>
-      <c r="D21" s="317" t="s">
+      <c r="D21" s="318" t="s">
         <v>517</v>
       </c>
       <c r="E21" s="189" t="s">
@@ -21981,8 +21716,8 @@
       <c r="B22" s="152" t="s">
         <v>275</v>
       </c>
-      <c r="C22" s="322"/>
-      <c r="D22" s="318"/>
+      <c r="C22" s="323"/>
+      <c r="D22" s="319"/>
       <c r="E22" s="264"/>
       <c r="P22" s="145">
         <v>4.9000000000000004</v>
@@ -22027,13 +21762,13 @@
       <c r="B24" s="150" t="s">
         <v>518</v>
       </c>
-      <c r="C24" s="321">
+      <c r="C24" s="322">
         <v>110</v>
       </c>
-      <c r="D24" s="319">
+      <c r="D24" s="320">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E24" s="319">
+      <c r="E24" s="320">
         <v>28.047042804386201</v>
       </c>
       <c r="H24" s="136">
@@ -22055,9 +21790,9 @@
       <c r="B25" s="152" t="s">
         <v>282</v>
       </c>
-      <c r="C25" s="322"/>
-      <c r="D25" s="320"/>
-      <c r="E25" s="320"/>
+      <c r="C25" s="323"/>
+      <c r="D25" s="321"/>
+      <c r="E25" s="321"/>
       <c r="P25" s="145">
         <f>P22/P23</f>
         <v>13.611111111111112</v>
@@ -22091,13 +21826,13 @@
       <c r="B27" s="150" t="s">
         <v>286</v>
       </c>
-      <c r="C27" s="321">
+      <c r="C27" s="322">
         <v>267</v>
       </c>
-      <c r="D27" s="321">
+      <c r="D27" s="322">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E27" s="321">
+      <c r="E27" s="322">
         <v>26.809100000000001</v>
       </c>
       <c r="H27" s="136">
@@ -22135,9 +21870,9 @@
       <c r="B28" s="152" t="s">
         <v>290</v>
       </c>
-      <c r="C28" s="322"/>
-      <c r="D28" s="322"/>
-      <c r="E28" s="322"/>
+      <c r="C28" s="323"/>
+      <c r="D28" s="323"/>
+      <c r="E28" s="323"/>
     </row>
     <row r="29" spans="2:28" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="148" t="s">
@@ -24309,7 +24044,7 @@
   <dimension ref="B1:J25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25204,15 +24939,15 @@
         <v>458</v>
       </c>
       <c r="D47" s="211"/>
-      <c r="E47" s="328" t="s">
+      <c r="E47" s="329" t="s">
         <v>459</v>
       </c>
-      <c r="F47" s="329"/>
-      <c r="G47" s="330" t="s">
+      <c r="F47" s="330"/>
+      <c r="G47" s="331" t="s">
         <v>460</v>
       </c>
-      <c r="H47" s="330"/>
-      <c r="I47" s="330"/>
+      <c r="H47" s="331"/>
+      <c r="I47" s="331"/>
       <c r="L47" s="141"/>
     </row>
     <row r="48" spans="2:12" ht="28.5" x14ac:dyDescent="0.25">
@@ -25227,10 +24962,10 @@
       <c r="F48" s="216" t="s">
         <v>462</v>
       </c>
-      <c r="G48" s="331" t="s">
+      <c r="G48" s="332" t="s">
         <v>463</v>
       </c>
-      <c r="H48" s="331"/>
+      <c r="H48" s="332"/>
       <c r="I48" s="217" t="s">
         <v>462</v>
       </c>
@@ -26514,7 +26249,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N26" sqref="M26:N28"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26634,7 +26369,7 @@
         <v>582</v>
       </c>
       <c r="H9" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
       <c r="I9" s="313"/>
       <c r="J9" s="313"/>
@@ -26659,7 +26394,7 @@
         <v>582</v>
       </c>
       <c r="H10" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
       <c r="I10" s="313"/>
       <c r="J10" s="313"/>
@@ -26684,7 +26419,7 @@
         <v>582</v>
       </c>
       <c r="H11" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
       <c r="I11" s="313"/>
       <c r="J11" s="313"/>
@@ -26709,7 +26444,7 @@
         <v>582</v>
       </c>
       <c r="H12" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
       <c r="I12" s="313"/>
       <c r="J12" s="313"/>
@@ -26734,7 +26469,7 @@
         <v>582</v>
       </c>
       <c r="H13" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
       <c r="I13" s="313"/>
       <c r="J13" s="313"/>
@@ -26759,7 +26494,7 @@
         <v>582</v>
       </c>
       <c r="H14" s="313" t="s">
-        <v>570</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -26799,13 +26534,13 @@
   <sheetPr codeName="Sheet30">
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:AC36"/>
+  <dimension ref="A1:AD36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="6" ySplit="7" topLeftCell="M8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
+      <selection pane="bottomRight" activeCell="K36" sqref="K36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -26816,21 +26551,22 @@
     <col min="4" max="4" width="8.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
-    <col min="7" max="9" width="9.140625" style="3"/>
-    <col min="10" max="10" width="24.85546875" style="3" customWidth="1"/>
-    <col min="11" max="17" width="9.140625" style="3"/>
-    <col min="18" max="18" width="7.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="7.5703125" style="3" customWidth="1"/>
-    <col min="20" max="21" width="7.85546875" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="10" width="9.140625" style="3"/>
+    <col min="11" max="11" width="24.85546875" style="3" customWidth="1"/>
+    <col min="12" max="18" width="9.140625" style="3"/>
+    <col min="19" max="19" width="7.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="7.5703125" style="3" customWidth="1"/>
+    <col min="21" max="22" width="7.85546875" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="9"/>
       <c r="G1" s="31"/>
-    </row>
-    <row r="2" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="31"/>
+    </row>
+    <row r="2" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -26838,14 +26574,13 @@
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
-    </row>
-    <row r="3" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G3" s="92" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="92" t="s">
-        <v>146</v>
-      </c>
+      <c r="H3" s="92"/>
       <c r="I3" s="92" t="s">
         <v>146</v>
       </c>
@@ -26859,13 +26594,13 @@
         <v>146</v>
       </c>
       <c r="M3" s="92" t="s">
+        <v>146</v>
+      </c>
+      <c r="N3" s="92" t="s">
         <v>150</v>
       </c>
-      <c r="N3" s="92" t="s">
+      <c r="O3" s="92" t="s">
         <v>192</v>
-      </c>
-      <c r="O3" s="92" t="s">
-        <v>194</v>
       </c>
       <c r="P3" s="92" t="s">
         <v>194</v>
@@ -26873,19 +26608,20 @@
       <c r="Q3" s="92" t="s">
         <v>194</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R3" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="H4" s="39" t="s">
-        <v>149</v>
-      </c>
+      <c r="H4" s="39"/>
       <c r="I4" s="39" t="s">
         <v>149</v>
       </c>
@@ -26899,13 +26635,13 @@
         <v>149</v>
       </c>
       <c r="M4" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="N4" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="O4" s="39" t="s">
         <v>193</v>
-      </c>
-      <c r="O4" s="39" t="s">
-        <v>195</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>195</v>
@@ -26913,8 +26649,8 @@
       <c r="Q4" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="R4" s="90" t="s">
-        <v>145</v>
+      <c r="R4" s="39" t="s">
+        <v>195</v>
       </c>
       <c r="S4" s="90" t="s">
         <v>145</v>
@@ -26925,32 +26661,36 @@
       <c r="U4" s="90" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V4" s="90" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="39"/>
+      <c r="I5" s="39">
         <v>2017</v>
       </c>
-      <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="O5" s="3" t="str">
+      <c r="M5" s="39"/>
+      <c r="P5" s="3" t="str">
         <f>EB_Exist!A9</f>
         <v>CO2SPIFC</v>
       </c>
-      <c r="P5" s="3" t="str">
+      <c r="Q5" s="3" t="str">
         <f>EB_Exist!A26</f>
         <v>CO2SPIFM</v>
       </c>
-      <c r="Q5" s="3" t="str">
+      <c r="R5" s="3" t="str">
         <f>EB_Exist!A10</f>
         <v>CH4S</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="316" t="s">
         <v>591</v>
       </c>
@@ -26962,17 +26702,18 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="39"/>
-      <c r="O6" s="31" t="s">
-        <v>124</v>
-      </c>
+      <c r="M6" s="39"/>
       <c r="P6" s="31" t="s">
         <v>124</v>
       </c>
       <c r="Q6" s="31" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="R6" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>552</v>
       </c>
@@ -26991,42 +26732,42 @@
       <c r="G7" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="314" t="s">
+      <c r="H7" s="39" t="s">
+        <v>600</v>
+      </c>
+      <c r="I7" s="314" t="s">
         <v>584</v>
       </c>
-      <c r="I7" s="314" t="s">
+      <c r="J7" s="314" t="s">
         <v>585</v>
       </c>
-      <c r="J7" s="314" t="s">
+      <c r="K7" s="314" t="s">
         <v>586</v>
       </c>
-      <c r="K7" s="314" t="s">
+      <c r="L7" s="314" t="s">
         <v>587</v>
       </c>
-      <c r="L7" s="314" t="s">
+      <c r="M7" s="314" t="s">
         <v>588</v>
       </c>
-      <c r="M7" s="31" t="str">
-        <f t="shared" ref="M7" si="0">IFERROR(REPLACE(M4,SEARCH("-",M4),1,"~"),M4)</f>
+      <c r="N7" s="31" t="str">
+        <f t="shared" ref="N7" si="0">IFERROR(REPLACE(N4,SEARCH("-",N4),1,"~"),N4)</f>
         <v>NCAP_FOM</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="O7" s="39" t="s">
         <v>193</v>
-      </c>
-      <c r="O7" s="92" t="str">
-        <f>"ENV_ACT~"&amp;O5</f>
-        <v>ENV_ACT~CO2SPIFC</v>
       </c>
       <c r="P7" s="92" t="str">
         <f>"ENV_ACT~"&amp;P5</f>
-        <v>ENV_ACT~CO2SPIFM</v>
+        <v>ENV_ACT~CO2SPIFC</v>
       </c>
       <c r="Q7" s="92" t="str">
         <f>"ENV_ACT~"&amp;Q5</f>
+        <v>ENV_ACT~CO2SPIFM</v>
+      </c>
+      <c r="R7" s="92" t="str">
+        <f>"ENV_ACT~"&amp;R5</f>
         <v>ENV_ACT~CH4S</v>
-      </c>
-      <c r="R7" s="31" t="s">
-        <v>145</v>
       </c>
       <c r="S7" s="31" t="s">
         <v>145</v>
@@ -27037,11 +26778,17 @@
       <c r="U7" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="V7" s="3" t="s">
+      <c r="V7" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="W7" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="X7" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="str">
         <f>Processes_BASE!B9</f>
         <v>XINDBIO</v>
@@ -27068,11 +26815,12 @@
       <c r="J8" s="30"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
-      <c r="N8" s="3">
+      <c r="M8" s="30"/>
+      <c r="O8" s="3">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="31" t="str">
         <f>Processes_BASE!B10</f>
@@ -27092,15 +26840,16 @@
       </c>
       <c r="F9" s="99"/>
       <c r="G9" s="93"/>
-      <c r="M9" s="89"/>
+      <c r="H9" s="93"/>
       <c r="N9" s="89"/>
-      <c r="R9" s="94">
+      <c r="O9" s="89"/>
+      <c r="S9" s="94">
         <f>EB_Exist!K6/EB_Exist!F5</f>
         <v>20.407577497129733</v>
       </c>
-      <c r="S9" s="3"/>
-    </row>
-    <row r="10" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="E10" s="99" t="str">
         <f>RES_Cr!E2</f>
@@ -27113,17 +26862,18 @@
       <c r="J10" s="93"/>
       <c r="K10" s="93"/>
       <c r="L10" s="93"/>
-      <c r="M10" s="3"/>
+      <c r="M10" s="93"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
-      <c r="S10" s="131">
+      <c r="R10" s="3"/>
+      <c r="T10" s="131">
         <f>EB_Exist!K7/EB_Exist!F5</f>
         <v>4.0379205223880605</v>
       </c>
     </row>
-    <row r="11" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="E11" s="98" t="str">
         <f>RES_Cr!F2</f>
@@ -27135,17 +26885,18 @@
       <c r="J11" s="93"/>
       <c r="K11" s="93"/>
       <c r="L11" s="93"/>
-      <c r="M11" s="3"/>
+      <c r="M11" s="93"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
-      <c r="T11" s="131">
+      <c r="R11" s="3"/>
+      <c r="U11" s="131">
         <f>EB_Exist!K8/EB_Exist!F5</f>
         <v>12.360988518943744</v>
       </c>
     </row>
-    <row r="12" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -27157,35 +26908,41 @@
       </c>
       <c r="G12" s="93"/>
       <c r="H12" s="93">
+        <v>2</v>
+      </c>
+      <c r="I12" s="93">
         <f>EB_Exist!K5</f>
         <v>4.8570000000000002</v>
       </c>
-      <c r="I12" s="93">
-        <f>H12</f>
+      <c r="J12" s="93">
+        <f>I12</f>
         <v>4.8570000000000002</v>
       </c>
-      <c r="J12" s="93">
+      <c r="K12" s="93">
         <v>4</v>
       </c>
-      <c r="K12" s="93">
+      <c r="L12" s="93">
         <v>3</v>
       </c>
-      <c r="L12" s="93">
+      <c r="M12" s="93">
         <v>0</v>
       </c>
-      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="89">
+      <c r="O12" s="3"/>
+      <c r="P12" s="89">
         <f>EB_Exist!F9</f>
         <v>3225</v>
       </c>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="126">
+      <c r="Q12" s="89"/>
+      <c r="R12" s="126">
         <f>EB_Exist!F10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="31" t="str">
         <f>RES_Cr!R15</f>
@@ -27210,22 +26967,23 @@
       <c r="J13" s="93"/>
       <c r="K13" s="93"/>
       <c r="L13" s="93"/>
-      <c r="M13" s="3"/>
+      <c r="M13" s="93"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="128">
+      <c r="R13" s="3"/>
+      <c r="S13" s="128">
         <v>4.4800000000000004</v>
       </c>
-      <c r="S13" s="128"/>
       <c r="T13" s="128"/>
       <c r="U13" s="128"/>
-      <c r="V13" s="26">
+      <c r="V13" s="128"/>
+      <c r="W13" s="26">
         <v>2031</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -27246,14 +27004,15 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="128"/>
-      <c r="S14" s="128">
+      <c r="R14" s="3"/>
+      <c r="S14" s="128"/>
+      <c r="T14" s="128">
         <v>3.89</v>
       </c>
-      <c r="T14" s="128"/>
       <c r="U14" s="128"/>
-    </row>
-    <row r="15" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="128"/>
+    </row>
+    <row r="15" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -27273,14 +27032,15 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="3"/>
-      <c r="R15" s="128"/>
+      <c r="R15" s="3"/>
       <c r="S15" s="128"/>
-      <c r="T15" s="128">
+      <c r="T15" s="128"/>
+      <c r="U15" s="128">
         <v>8.64</v>
       </c>
-      <c r="U15" s="128"/>
-    </row>
-    <row r="16" spans="1:22" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V15" s="128"/>
+    </row>
+    <row r="16" spans="1:24" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -27301,35 +27061,39 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3"/>
-      <c r="R16" s="128"/>
+      <c r="R16" s="3"/>
       <c r="S16" s="128"/>
       <c r="T16" s="128"/>
-      <c r="U16" s="128">
+      <c r="U16" s="128"/>
+      <c r="V16" s="128">
         <v>7.72</v>
       </c>
     </row>
-    <row r="17" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="99" t="str">
         <f>RES_Cr!T2</f>
         <v>IFACR</v>
       </c>
-      <c r="M17" s="129">
-        <f>2%*N17</f>
+      <c r="N17" s="129">
+        <f>2%*O17</f>
         <v>201.44</v>
       </c>
-      <c r="N17" s="129">
+      <c r="O17" s="129">
         <v>10072</v>
       </c>
-      <c r="O17" s="129">
+      <c r="P17" s="129">
         <v>2102</v>
       </c>
-      <c r="P17" s="129"/>
-      <c r="Q17" s="129">
-        <f>Q12*0.8</f>
+      <c r="Q17" s="129"/>
+      <c r="R17" s="129">
+        <f>R12*0.8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="str">
         <f>RES_Cr!R22</f>
         <v>IFCEAFB-N</v>
@@ -27353,77 +27117,81 @@
       <c r="J18" s="93"/>
       <c r="K18" s="93"/>
       <c r="L18" s="93"/>
-      <c r="R18" s="128">
+      <c r="M18" s="93"/>
+      <c r="S18" s="128">
         <v>1.55</v>
       </c>
-      <c r="S18" s="128"/>
       <c r="T18" s="128"/>
       <c r="U18" s="128"/>
-      <c r="V18" s="26">
+      <c r="V18" s="128"/>
+      <c r="W18" s="26">
         <v>2031</v>
       </c>
     </row>
-    <row r="19" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="99" t="str">
         <f t="shared" ref="E19:E21" si="1">E14</f>
         <v>IISCOA</v>
       </c>
       <c r="F19" s="98"/>
-      <c r="R19" s="128"/>
-      <c r="S19" s="128">
+      <c r="S19" s="128"/>
+      <c r="T19" s="128">
         <v>2.33</v>
       </c>
-      <c r="T19" s="128"/>
       <c r="U19" s="128"/>
-    </row>
-    <row r="20" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="128"/>
+    </row>
+    <row r="20" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="99" t="str">
         <f t="shared" si="1"/>
         <v>IFAELC</v>
       </c>
       <c r="F20" s="26"/>
-      <c r="R20" s="128"/>
       <c r="S20" s="128"/>
-      <c r="T20" s="128">
+      <c r="T20" s="128"/>
+      <c r="U20" s="128">
         <v>8.64</v>
       </c>
-      <c r="U20" s="128"/>
-    </row>
-    <row r="21" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="128"/>
+    </row>
+    <row r="21" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="99" t="str">
         <f t="shared" si="1"/>
         <v>IFACHA</v>
       </c>
       <c r="F21" s="38"/>
-      <c r="R21" s="128"/>
       <c r="S21" s="128"/>
       <c r="T21" s="128"/>
-      <c r="U21" s="128">
+      <c r="U21" s="128"/>
+      <c r="V21" s="128">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="99" t="str">
         <f>F17</f>
         <v>IFACR</v>
       </c>
-      <c r="M22" s="129">
-        <f>2%*N22</f>
+      <c r="N22" s="129">
+        <f>2%*O22</f>
         <v>221.58</v>
       </c>
-      <c r="N22" s="129">
+      <c r="O22" s="129">
         <v>11079</v>
       </c>
-      <c r="O22" s="129">
+      <c r="P22" s="129">
         <v>933</v>
       </c>
-      <c r="P22" s="129"/>
-      <c r="Q22" s="129">
-        <f>Q17*0.8</f>
+      <c r="Q22" s="129"/>
+      <c r="R22" s="129">
+        <f>R17*0.8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="X22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="str">
         <f>Processes_BASE!B13</f>
         <v>IFMEAF-E</v>
@@ -27442,21 +27210,21 @@
       </c>
       <c r="F23" s="99"/>
       <c r="G23" s="93"/>
-      <c r="H23" s="26"/>
+      <c r="H23" s="93"/>
       <c r="I23" s="26"/>
       <c r="J23" s="26"/>
       <c r="K23" s="26"/>
       <c r="L23" s="26"/>
-      <c r="M23" s="89"/>
+      <c r="M23" s="26"/>
       <c r="N23" s="89"/>
-      <c r="O23" s="26"/>
+      <c r="O23" s="89"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
-      <c r="R23" s="94">
+      <c r="R23" s="26"/>
+      <c r="S23" s="94">
         <f>EB_Exist!K23/EB_Exist!F22</f>
         <v>9.8455813953488391</v>
       </c>
-      <c r="T23" s="26"/>
       <c r="U23" s="26"/>
       <c r="V23" s="26"/>
       <c r="W23" s="26"/>
@@ -27466,8 +27234,9 @@
       <c r="AA23" s="26"/>
       <c r="AB23" s="26"/>
       <c r="AC23" s="26"/>
-    </row>
-    <row r="24" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD23" s="26"/>
+    </row>
+    <row r="24" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -27482,12 +27251,12 @@
       <c r="J24" s="93"/>
       <c r="K24" s="93"/>
       <c r="L24" s="93"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="131">
+      <c r="M24" s="93"/>
+      <c r="S24" s="26"/>
+      <c r="T24" s="131">
         <f>EB_Exist!K24/EB_Exist!F22</f>
         <v>3.2818604651162797</v>
       </c>
-      <c r="T24" s="26"/>
       <c r="U24" s="26"/>
       <c r="V24" s="26"/>
       <c r="W24" s="26"/>
@@ -27497,8 +27266,9 @@
       <c r="AA24" s="26"/>
       <c r="AB24" s="26"/>
       <c r="AC24" s="26"/>
-    </row>
-    <row r="25" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD24" s="26"/>
+    </row>
+    <row r="25" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -27513,13 +27283,13 @@
       <c r="J25" s="93"/>
       <c r="K25" s="93"/>
       <c r="L25" s="93"/>
-      <c r="R25" s="26"/>
+      <c r="M25" s="93"/>
       <c r="S25" s="26"/>
-      <c r="T25" s="131">
+      <c r="T25" s="26"/>
+      <c r="U25" s="131">
         <f>EB_Exist!K25/EB_Exist!F22</f>
         <v>12.96</v>
       </c>
-      <c r="U25" s="26"/>
       <c r="V25" s="26"/>
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
@@ -27528,53 +27298,56 @@
       <c r="AA25" s="26"/>
       <c r="AB25" s="26"/>
       <c r="AC25" s="26"/>
-    </row>
-    <row r="26" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AD25" s="26"/>
+    </row>
+    <row r="26" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="99"/>
       <c r="F26" s="98" t="str">
         <f>RES_Mn!O2</f>
         <v>IFAMN</v>
       </c>
       <c r="G26" s="93"/>
-      <c r="H26" s="93">
+      <c r="I26" s="93">
         <f>EB_Exist!K22*0.9</f>
         <v>0.68490000000000006</v>
       </c>
-      <c r="I26" s="93">
-        <f>H26</f>
+      <c r="J26" s="93">
+        <f>I26</f>
         <v>0.68490000000000006</v>
       </c>
-      <c r="J26" s="93">
+      <c r="K26" s="93">
         <v>0.3</v>
       </c>
-      <c r="K26" s="93">
+      <c r="L26" s="93">
         <v>0.1</v>
       </c>
-      <c r="L26" s="93">
+      <c r="M26" s="93">
         <v>0</v>
       </c>
-      <c r="P26" s="89">
+      <c r="Q26" s="89">
         <f>EB_Exist!F26</f>
         <v>3225</v>
       </c>
-      <c r="Q26" s="126">
+      <c r="R26" s="126">
         <f>EB_Exist!F27</f>
         <v>0</v>
       </c>
-      <c r="R26" s="26"/>
       <c r="S26" s="26"/>
       <c r="T26" s="26"/>
       <c r="U26" s="26"/>
       <c r="V26" s="26"/>
       <c r="W26" s="26"/>
-      <c r="X26" s="26"/>
+      <c r="X26" s="26">
+        <v>1</v>
+      </c>
       <c r="Y26" s="26"/>
       <c r="Z26" s="26"/>
       <c r="AA26" s="26"/>
       <c r="AB26" s="26"/>
       <c r="AC26" s="26"/>
-    </row>
-    <row r="27" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD26" s="26"/>
+    </row>
+    <row r="27" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="str">
         <f>RES_Mn!M15</f>
         <v>IFMEAF-N</v>
@@ -27598,38 +27371,38 @@
       <c r="J27" s="93"/>
       <c r="K27" s="93"/>
       <c r="L27" s="93"/>
-      <c r="R27" s="128">
-        <f>R23/2</f>
+      <c r="M27" s="93"/>
+      <c r="S27" s="128">
+        <f>S23/2</f>
         <v>4.9227906976744196</v>
       </c>
-      <c r="S27" s="128"/>
       <c r="T27" s="128"/>
       <c r="U27" s="128"/>
-      <c r="V27" s="26">
+      <c r="V27" s="128"/>
+      <c r="W27" s="26">
         <v>2031</v>
       </c>
-      <c r="W27" s="26"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
       <c r="Z27" s="26"/>
       <c r="AA27" s="26"/>
       <c r="AB27" s="26"/>
       <c r="AC27" s="26"/>
-    </row>
-    <row r="28" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD27" s="26"/>
+    </row>
+    <row r="28" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="99" t="str">
         <f>RES_Mn!E2</f>
         <v>IISCOA</v>
       </c>
       <c r="F28" s="98"/>
-      <c r="R28" s="128"/>
-      <c r="S28" s="258">
-        <f>S24</f>
+      <c r="S28" s="128"/>
+      <c r="T28" s="258">
+        <f>T24</f>
         <v>3.2818604651162797</v>
       </c>
-      <c r="T28" s="128"/>
       <c r="U28" s="128"/>
-      <c r="V28" s="26"/>
+      <c r="V28" s="128"/>
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
@@ -27637,21 +27410,21 @@
       <c r="AA28" s="26"/>
       <c r="AB28" s="26"/>
       <c r="AC28" s="26"/>
-    </row>
-    <row r="29" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD28" s="26"/>
+    </row>
+    <row r="29" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="99" t="str">
         <f>RES_Mn!F2</f>
         <v>IFAELC</v>
       </c>
       <c r="F29" s="26"/>
-      <c r="R29" s="128"/>
       <c r="S29" s="128"/>
-      <c r="T29" s="128">
+      <c r="T29" s="128"/>
+      <c r="U29" s="128">
         <f>EB_Exist!U55</f>
         <v>10.08</v>
       </c>
-      <c r="U29" s="128"/>
-      <c r="V29" s="26"/>
+      <c r="V29" s="128"/>
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
       <c r="Y29" s="26"/>
@@ -27659,21 +27432,21 @@
       <c r="AA29" s="26"/>
       <c r="AB29" s="26"/>
       <c r="AC29" s="26"/>
-    </row>
-    <row r="30" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD29" s="26"/>
+    </row>
+    <row r="30" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="99" t="str">
         <f>RES_Mn!G2</f>
         <v>IFACHA</v>
       </c>
       <c r="F30" s="38"/>
-      <c r="R30" s="128"/>
       <c r="S30" s="128"/>
       <c r="T30" s="128"/>
-      <c r="U30" s="128">
-        <f>R27*1.1</f>
+      <c r="U30" s="128"/>
+      <c r="V30" s="128">
+        <f>S27*1.1</f>
         <v>5.415069767441862</v>
       </c>
-      <c r="V30" s="26"/>
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
@@ -27681,29 +27454,33 @@
       <c r="AA30" s="26"/>
       <c r="AB30" s="26"/>
       <c r="AC30" s="26"/>
-    </row>
-    <row r="31" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD30" s="26"/>
+    </row>
+    <row r="31" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="99" t="str">
         <f>RES_Mn!O2</f>
         <v>IFAMN</v>
       </c>
-      <c r="M31" s="129">
-        <f>2%*N31</f>
+      <c r="N31" s="129">
+        <f>2%*O31</f>
         <v>201.44</v>
       </c>
-      <c r="N31" s="129">
+      <c r="O31" s="129">
         <v>10072</v>
       </c>
-      <c r="O31" s="129"/>
-      <c r="P31" s="129">
+      <c r="P31" s="129"/>
+      <c r="Q31" s="129">
         <v>2102</v>
       </c>
-      <c r="Q31" s="129">
-        <f>Q26*0.8</f>
+      <c r="R31" s="129">
+        <f>R26*0.8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:29" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X31" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:30" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="31" t="str">
         <f>RES_Mn!M22</f>
         <v>IFMEAFB-N</v>
@@ -27727,78 +27504,82 @@
       <c r="J32" s="93"/>
       <c r="K32" s="93"/>
       <c r="L32" s="93"/>
-      <c r="R32" s="128">
-        <f>R23*0.25</f>
+      <c r="M32" s="93"/>
+      <c r="S32" s="128">
+        <f>S23*0.25</f>
         <v>2.4613953488372098</v>
       </c>
-      <c r="S32" s="128"/>
       <c r="T32" s="128"/>
       <c r="U32" s="128"/>
-      <c r="V32" s="26">
+      <c r="V32" s="128"/>
+      <c r="W32" s="26">
         <v>2031</v>
       </c>
     </row>
-    <row r="33" spans="5:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="99" t="str">
         <f>E28</f>
         <v>IISCOA</v>
       </c>
       <c r="F33" s="98"/>
-      <c r="R33" s="128"/>
-      <c r="S33" s="258">
-        <f>S24</f>
+      <c r="S33" s="128"/>
+      <c r="T33" s="258">
+        <f>T24</f>
         <v>3.2818604651162797</v>
       </c>
-      <c r="T33" s="128"/>
       <c r="U33" s="128"/>
-    </row>
-    <row r="34" spans="5:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V33" s="128"/>
+    </row>
+    <row r="34" spans="5:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="99" t="str">
         <f>E29</f>
         <v>IFAELC</v>
       </c>
       <c r="F34" s="26"/>
-      <c r="R34" s="128"/>
       <c r="S34" s="128"/>
-      <c r="T34" s="128">
-        <f>T29</f>
+      <c r="T34" s="128"/>
+      <c r="U34" s="128">
+        <f>U29</f>
         <v>10.08</v>
       </c>
-      <c r="U34" s="128"/>
-    </row>
-    <row r="35" spans="5:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V34" s="128"/>
+    </row>
+    <row r="35" spans="5:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="99" t="str">
         <f>E30</f>
         <v>IFACHA</v>
       </c>
       <c r="F35" s="38"/>
-      <c r="R35" s="128"/>
       <c r="S35" s="128"/>
       <c r="T35" s="128"/>
-      <c r="U35" s="128">
-        <f>R23*0.75*1.1</f>
+      <c r="U35" s="128"/>
+      <c r="V35" s="128">
+        <f>S23*0.75*1.1</f>
         <v>8.1226046511627938</v>
       </c>
     </row>
-    <row r="36" spans="5:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F36" s="99" t="str">
         <f>F31</f>
         <v>IFAMN</v>
       </c>
-      <c r="M36" s="129">
-        <f>2%*N36</f>
+      <c r="N36" s="129">
+        <f>2%*O36</f>
         <v>221.58</v>
       </c>
-      <c r="N36" s="129">
+      <c r="O36" s="129">
         <v>11079</v>
       </c>
-      <c r="O36" s="129"/>
-      <c r="P36" s="129">
+      <c r="P36" s="129"/>
+      <c r="Q36" s="129">
         <v>933</v>
       </c>
-      <c r="Q36" s="129">
-        <f>Q31*0.8</f>
+      <c r="R36" s="129">
+        <f>R31*0.8</f>
         <v>0</v>
+      </c>
+      <c r="X36" s="3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -27857,8 +27638,7 @@
       <c r="I5" t="s">
         <v>231</v>
       </c>
-      <c r="J5" t="b" cm="1">
-        <f t="array" ref="J5">[2]!pamsindex</f>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Iron and steel updates
Made Saldanha zero capacity after 2020. They are not likely to restart. And we need to add hydrogen investment for them to go hydrogen.

Have added FOM costs to all steel production techs - it was missing.
Have added TLIFE to new I&S techs. This was missing. Whoops.
Added to FERROALLOYS AS WELL.
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-FA.xlsx
+++ b/vt_REGION1_IND-FA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB710B14-BAC2-4E5C-BD4B-187980ADC5CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CCBFCD-9832-4B51-BEA7-72A67B457255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="818" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="818" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About and Log" sheetId="64" r:id="rId1"/>
@@ -939,7 +939,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="632">
   <si>
     <t>Comment</t>
   </si>
@@ -3164,6 +3164,9 @@
   </si>
   <si>
     <t>Coal feedstock</t>
+  </si>
+  <si>
+    <t>NCAP_TLIFE</t>
   </si>
 </sst>
 </file>
@@ -5289,6 +5292,33 @@
     <xf numFmtId="0" fontId="63" fillId="22" borderId="0" xfId="23" applyFont="1" applyFill="1"/>
     <xf numFmtId="169" fontId="53" fillId="0" borderId="0" xfId="23" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="53" fillId="23" borderId="0" xfId="23" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="7" borderId="41" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="7" borderId="43" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="41" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="43" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5307,31 +5337,10 @@
     <xf numFmtId="166" fontId="60" fillId="0" borderId="49" xfId="23" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="50" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="49" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="7" borderId="41" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="7" borderId="43" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="41" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="43" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="68" fillId="11" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5345,12 +5354,6 @@
     </xf>
     <xf numFmtId="0" fontId="68" fillId="12" borderId="0" xfId="23" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="78">
@@ -21993,7 +21996,7 @@
         <v>IFACR</v>
       </c>
       <c r="H9" s="130">
-        <f>'Process Input'!Q11</f>
+        <f>'Process Input'!R11</f>
         <v>12.360988518943744</v>
       </c>
       <c r="I9" s="94">
@@ -22101,7 +22104,7 @@
       <c r="E2" s="309"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="349" t="s">
+      <c r="B3" s="343" t="s">
         <v>241</v>
       </c>
       <c r="C3" s="139" t="s">
@@ -22110,21 +22113,21 @@
       <c r="E3" s="310"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="349"/>
+      <c r="B4" s="343"/>
       <c r="C4" s="139" t="s">
         <v>243</v>
       </c>
       <c r="E4" s="310"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="350"/>
+      <c r="B5" s="344"/>
       <c r="C5" s="141" t="s">
         <v>244</v>
       </c>
       <c r="E5" s="310"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="351" t="s">
+      <c r="B6" s="345" t="s">
         <v>245</v>
       </c>
       <c r="C6" s="142" t="s">
@@ -22133,21 +22136,21 @@
       <c r="E6" s="310"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="352"/>
+      <c r="B7" s="346"/>
       <c r="C7" s="142" t="s">
         <v>247</v>
       </c>
       <c r="E7" s="310"/>
     </row>
     <row r="8" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="353"/>
+      <c r="B8" s="347"/>
       <c r="C8" s="143" t="s">
         <v>248</v>
       </c>
       <c r="E8" s="310"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="351" t="s">
+      <c r="B9" s="345" t="s">
         <v>249</v>
       </c>
       <c r="C9" s="142" t="s">
@@ -22156,21 +22159,21 @@
       <c r="E9" s="310"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="352"/>
+      <c r="B10" s="346"/>
       <c r="C10" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E10" s="310"/>
     </row>
     <row r="11" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="353"/>
+      <c r="B11" s="347"/>
       <c r="C11" s="143" t="s">
         <v>252</v>
       </c>
       <c r="E11" s="310"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="351" t="s">
+      <c r="B12" s="345" t="s">
         <v>253</v>
       </c>
       <c r="C12" s="142" t="s">
@@ -22179,14 +22182,14 @@
       <c r="E12" s="310"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="352"/>
+      <c r="B13" s="346"/>
       <c r="C13" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E13" s="310"/>
     </row>
     <row r="14" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="353"/>
+      <c r="B14" s="347"/>
       <c r="C14" s="143" t="s">
         <v>254</v>
       </c>
@@ -22293,10 +22296,10 @@
       <c r="B21" s="318" t="s">
         <v>269</v>
       </c>
-      <c r="C21" s="345">
+      <c r="C21" s="341">
         <v>1200</v>
       </c>
-      <c r="D21" s="339" t="s">
+      <c r="D21" s="348" t="s">
         <v>511</v>
       </c>
       <c r="E21" s="319" t="s">
@@ -22323,8 +22326,8 @@
       <c r="B22" s="320" t="s">
         <v>271</v>
       </c>
-      <c r="C22" s="346"/>
-      <c r="D22" s="340"/>
+      <c r="C22" s="342"/>
+      <c r="D22" s="349"/>
       <c r="E22" s="321"/>
       <c r="Q22" s="144">
         <v>4.9000000000000004</v>
@@ -22369,13 +22372,13 @@
       <c r="B24" s="318" t="s">
         <v>512</v>
       </c>
-      <c r="C24" s="345">
+      <c r="C24" s="341">
         <v>110</v>
       </c>
-      <c r="D24" s="341">
+      <c r="D24" s="350">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E24" s="343">
+      <c r="E24" s="352">
         <v>28.047042804386201</v>
       </c>
       <c r="H24" s="135">
@@ -22397,9 +22400,9 @@
       <c r="B25" s="320" t="s">
         <v>278</v>
       </c>
-      <c r="C25" s="346"/>
-      <c r="D25" s="342"/>
-      <c r="E25" s="344"/>
+      <c r="C25" s="342"/>
+      <c r="D25" s="351"/>
+      <c r="E25" s="353"/>
       <c r="Q25" s="144">
         <f>Q22/Q23</f>
         <v>13.611111111111112</v>
@@ -22433,13 +22436,13 @@
       <c r="B27" s="318" t="s">
         <v>282</v>
       </c>
-      <c r="C27" s="345">
+      <c r="C27" s="341">
         <v>267</v>
       </c>
-      <c r="D27" s="345">
+      <c r="D27" s="341">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E27" s="347">
+      <c r="E27" s="354">
         <v>26.809100000000001</v>
       </c>
       <c r="H27" s="135">
@@ -22478,9 +22481,9 @@
       <c r="B28" s="320" t="s">
         <v>286</v>
       </c>
-      <c r="C28" s="346"/>
-      <c r="D28" s="346"/>
-      <c r="E28" s="348"/>
+      <c r="C28" s="342"/>
+      <c r="D28" s="342"/>
+      <c r="E28" s="355"/>
     </row>
     <row r="29" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="316" t="s">
@@ -24598,6 +24601,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
@@ -24605,11 +24613,6 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q19" r:id="rId1" xr:uid="{8CFFA192-6679-4FBF-B0CE-9327F43C0D73}"/>
@@ -24985,7 +24988,7 @@
       <c r="E14" s="309"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="349" t="s">
+      <c r="B15" s="343" t="s">
         <v>241</v>
       </c>
       <c r="C15" s="139" t="s">
@@ -24994,21 +24997,21 @@
       <c r="E15" s="310"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="349"/>
+      <c r="B16" s="343"/>
       <c r="C16" s="139" t="s">
         <v>243</v>
       </c>
       <c r="E16" s="310"/>
     </row>
     <row r="17" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="350"/>
+      <c r="B17" s="344"/>
       <c r="C17" s="141" t="s">
         <v>244</v>
       </c>
       <c r="E17" s="310"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="351" t="s">
+      <c r="B18" s="345" t="s">
         <v>245</v>
       </c>
       <c r="C18" s="142" t="s">
@@ -25017,21 +25020,21 @@
       <c r="E18" s="310"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="352"/>
+      <c r="B19" s="346"/>
       <c r="C19" s="142" t="s">
         <v>247</v>
       </c>
       <c r="E19" s="310"/>
     </row>
     <row r="20" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="353"/>
+      <c r="B20" s="347"/>
       <c r="C20" s="143" t="s">
         <v>248</v>
       </c>
       <c r="E20" s="310"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="351" t="s">
+      <c r="B21" s="345" t="s">
         <v>249</v>
       </c>
       <c r="C21" s="142" t="s">
@@ -25040,21 +25043,21 @@
       <c r="E21" s="310"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="352"/>
+      <c r="B22" s="346"/>
       <c r="C22" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E22" s="310"/>
     </row>
     <row r="23" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="353"/>
+      <c r="B23" s="347"/>
       <c r="C23" s="143" t="s">
         <v>252</v>
       </c>
       <c r="E23" s="310"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="351" t="s">
+      <c r="B24" s="345" t="s">
         <v>253</v>
       </c>
       <c r="C24" s="142" t="s">
@@ -25063,14 +25066,14 @@
       <c r="E24" s="310"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="352"/>
+      <c r="B25" s="346"/>
       <c r="C25" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E25" s="310"/>
     </row>
     <row r="26" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="353"/>
+      <c r="B26" s="347"/>
       <c r="C26" s="143" t="s">
         <v>254</v>
       </c>
@@ -25158,10 +25161,10 @@
       <c r="B33" s="318" t="s">
         <v>269</v>
       </c>
-      <c r="C33" s="345">
+      <c r="C33" s="341">
         <v>1200</v>
       </c>
-      <c r="D33" s="339" t="s">
+      <c r="D33" s="348" t="s">
         <v>511</v>
       </c>
       <c r="E33" s="319" t="s">
@@ -25186,8 +25189,8 @@
       <c r="B34" s="320" t="s">
         <v>271</v>
       </c>
-      <c r="C34" s="346"/>
-      <c r="D34" s="340"/>
+      <c r="C34" s="342"/>
+      <c r="D34" s="349"/>
       <c r="E34" s="321"/>
     </row>
     <row r="35" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25218,13 +25221,13 @@
       <c r="B36" s="318" t="s">
         <v>512</v>
       </c>
-      <c r="C36" s="345">
+      <c r="C36" s="341">
         <v>110</v>
       </c>
-      <c r="D36" s="341">
+      <c r="D36" s="350">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E36" s="343">
+      <c r="E36" s="352">
         <v>28.047042804386201</v>
       </c>
       <c r="H36" s="135">
@@ -25239,9 +25242,9 @@
       <c r="B37" s="320" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="346"/>
-      <c r="D37" s="342"/>
-      <c r="E37" s="344"/>
+      <c r="C37" s="342"/>
+      <c r="D37" s="351"/>
+      <c r="E37" s="353"/>
     </row>
     <row r="38" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="316" t="s">
@@ -25265,13 +25268,13 @@
       <c r="B39" s="318" t="s">
         <v>282</v>
       </c>
-      <c r="C39" s="345">
+      <c r="C39" s="341">
         <v>267</v>
       </c>
-      <c r="D39" s="345">
+      <c r="D39" s="341">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E39" s="347">
+      <c r="E39" s="354">
         <v>26.809100000000001</v>
       </c>
       <c r="H39" s="135">
@@ -25296,9 +25299,9 @@
       <c r="B40" s="320" t="s">
         <v>286</v>
       </c>
-      <c r="C40" s="346"/>
-      <c r="D40" s="346"/>
-      <c r="E40" s="348"/>
+      <c r="C40" s="342"/>
+      <c r="D40" s="342"/>
+      <c r="E40" s="355"/>
     </row>
     <row r="41" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="316" t="s">
@@ -27808,18 +27811,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C33:C34"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
     <mergeCell ref="E39:E40"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C33:C34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B273" r:id="rId1" xr:uid="{422A1BB5-B0D8-4A2F-BF63-C584298D04BA}"/>
@@ -28570,15 +28573,15 @@
         <v>452</v>
       </c>
       <c r="D47" s="203"/>
-      <c r="E47" s="354" t="s">
+      <c r="E47" s="356" t="s">
         <v>453</v>
       </c>
-      <c r="F47" s="355"/>
-      <c r="G47" s="356" t="s">
+      <c r="F47" s="357"/>
+      <c r="G47" s="358" t="s">
         <v>454</v>
       </c>
-      <c r="H47" s="356"/>
-      <c r="I47" s="356"/>
+      <c r="H47" s="358"/>
+      <c r="I47" s="358"/>
       <c r="L47" s="140"/>
     </row>
     <row r="48" spans="2:12" ht="28.5" x14ac:dyDescent="0.25">
@@ -28593,10 +28596,10 @@
       <c r="F48" s="208" t="s">
         <v>456</v>
       </c>
-      <c r="G48" s="357" t="s">
+      <c r="G48" s="359" t="s">
         <v>457</v>
       </c>
-      <c r="H48" s="357"/>
+      <c r="H48" s="359"/>
       <c r="I48" s="209" t="s">
         <v>456</v>
       </c>
@@ -30165,13 +30168,13 @@
   <sheetPr codeName="Sheet30">
     <tabColor rgb="FF0000FF"/>
   </sheetPr>
-  <dimension ref="A1:Y36"/>
+  <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23:S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30184,17 +30187,17 @@
     <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
     <col min="7" max="9" width="9.140625" style="3"/>
     <col min="10" max="10" width="24.85546875" style="3" customWidth="1"/>
-    <col min="11" max="16" width="9.140625" style="3"/>
-    <col min="17" max="17" width="7.85546875" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="3"/>
+    <col min="11" max="17" width="9.140625" style="3"/>
+    <col min="18" max="18" width="7.85546875" style="3" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="9"/>
       <c r="G1" s="31"/>
     </row>
-    <row r="2" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2"/>
       <c r="G2" s="31"/>
       <c r="H2" s="31"/>
@@ -30203,7 +30206,7 @@
       <c r="K2" s="31"/>
       <c r="L2" s="31"/>
     </row>
-    <row r="3" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G3" s="92" t="s">
         <v>148</v>
       </c>
@@ -30228,17 +30231,18 @@
       <c r="N3" s="92" t="s">
         <v>192</v>
       </c>
-      <c r="O3" s="92" t="s">
-        <v>194</v>
-      </c>
+      <c r="O3" s="92"/>
       <c r="P3" s="92" t="s">
         <v>194</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="92" t="s">
+        <v>194</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="27"/>
       <c r="F4" s="27"/>
       <c r="G4" s="39" t="s">
@@ -30265,17 +30269,18 @@
       <c r="N4" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="O4" s="39" t="s">
-        <v>195</v>
-      </c>
+      <c r="O4" s="39"/>
       <c r="P4" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="Q4" s="90" t="s">
+      <c r="Q4" s="39" t="s">
+        <v>195</v>
+      </c>
+      <c r="R4" s="90" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" s="39" t="s">
         <v>27</v>
       </c>
@@ -30286,14 +30291,14 @@
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F6" s="303" t="s">
         <v>585</v>
       </c>
@@ -30305,14 +30310,14 @@
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="39"/>
-      <c r="O6" s="31" t="s">
-        <v>124</v>
-      </c>
       <c r="P6" s="31" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Q6" s="31" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>546</v>
       </c>
@@ -30353,25 +30358,28 @@
       <c r="N7" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="O7" s="92" t="str">
-        <f>"ENV_ACT~"&amp;O5</f>
-        <v>ENV_ACT~CO2SPIFC</v>
+      <c r="O7" s="39" t="s">
+        <v>631</v>
       </c>
       <c r="P7" s="92" t="str">
         <f>"ENV_ACT~"&amp;P5</f>
+        <v>ENV_ACT~CO2SPIFC</v>
+      </c>
+      <c r="Q7" s="92" t="str">
+        <f>"ENV_ACT~"&amp;Q5</f>
         <v>ENV_ACT~CO2SPIFM</v>
       </c>
-      <c r="Q7" s="31" t="s">
+      <c r="R7" s="31" t="s">
         <v>145</v>
       </c>
-      <c r="R7" s="3" t="s">
+      <c r="S7" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="S7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="str">
         <f>Processes_BASE!B9</f>
         <v>XINDBIO</v>
@@ -30402,7 +30410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="31" t="str">
         <f>Processes_BASE!B10</f>
@@ -30424,12 +30432,13 @@
       <c r="G9" s="93"/>
       <c r="M9" s="89"/>
       <c r="N9" s="89"/>
-      <c r="Q9" s="94">
+      <c r="O9" s="89"/>
+      <c r="R9" s="94">
         <f>EB_Exist!K6/EB_Exist!F5</f>
         <v>20.407577497129733</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="E10" s="99" t="str">
         <f>RES_Cr!E2</f>
@@ -30446,12 +30455,13 @@
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
-      <c r="Q10" s="130">
+      <c r="Q10" s="3"/>
+      <c r="R10" s="130">
         <f>EB_Exist!K7/EB_Exist!F5</f>
         <v>4.0379205223880605</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="E11" s="98" t="str">
         <f>RES_Cr!F2</f>
@@ -30467,12 +30477,13 @@
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
-      <c r="Q11" s="130">
+      <c r="Q11" s="3"/>
+      <c r="R11" s="130">
         <f>EB_Exist!K8/EB_Exist!F5</f>
         <v>12.360988518943744</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -30490,16 +30501,17 @@
       <c r="L12" s="93"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
-      <c r="O12" s="89">
+      <c r="O12" s="3"/>
+      <c r="P12" s="89">
         <f>EB_Exist!F9</f>
         <v>3225</v>
       </c>
-      <c r="P12" s="89"/>
-      <c r="S12" s="26">
+      <c r="Q12" s="89"/>
+      <c r="T12" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="31" t="str">
         <f>RES_Cr!R15</f>
@@ -30528,11 +30540,12 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="127">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="127">
         <v>4.4800000000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -30552,11 +30565,12 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
-      <c r="Q14" s="127">
+      <c r="Q14" s="3"/>
+      <c r="R14" s="127">
         <v>3.89</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -30575,11 +30589,12 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
-      <c r="Q15" s="127">
+      <c r="Q15" s="3"/>
+      <c r="R15" s="127">
         <v>8.64</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="26" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -30599,11 +30614,12 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
-      <c r="Q16" s="127">
+      <c r="Q16" s="3"/>
+      <c r="R16" s="127">
         <v>7.72</v>
       </c>
     </row>
-    <row r="17" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="99" t="str">
         <f>RES_Cr!T2</f>
         <v>IFACR</v>
@@ -30616,17 +30632,20 @@
         <v>10072</v>
       </c>
       <c r="O17" s="128">
+        <v>20</v>
+      </c>
+      <c r="P17" s="128">
         <v>2102</v>
       </c>
-      <c r="P17" s="128"/>
-      <c r="R17" s="26">
+      <c r="Q17" s="128"/>
+      <c r="S17" s="26">
         <v>2025</v>
       </c>
-      <c r="S17" s="3">
+      <c r="T17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="31" t="str">
         <f>RES_Cr!R22</f>
         <v>IFCEAFB-N</v>
@@ -30650,41 +30669,41 @@
       <c r="J18" s="93"/>
       <c r="K18" s="93"/>
       <c r="L18" s="93"/>
-      <c r="Q18" s="127">
+      <c r="R18" s="127">
         <v>1.55</v>
       </c>
     </row>
-    <row r="19" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="99" t="str">
         <f t="shared" ref="E19:E21" si="1">E14</f>
         <v>INDCMU</v>
       </c>
       <c r="F19" s="98"/>
-      <c r="Q19" s="127">
+      <c r="R19" s="127">
         <v>2.33</v>
       </c>
     </row>
-    <row r="20" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E20" s="99" t="str">
         <f t="shared" si="1"/>
         <v>IFAELC</v>
       </c>
       <c r="F20" s="26"/>
-      <c r="Q20" s="127">
+      <c r="R20" s="127">
         <v>8.64</v>
       </c>
     </row>
-    <row r="21" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E21" s="99" t="str">
         <f t="shared" si="1"/>
         <v>IFACHA</v>
       </c>
       <c r="F21" s="38"/>
-      <c r="Q21" s="127">
+      <c r="R21" s="127">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" s="99" t="str">
         <f>F17</f>
         <v>IFACR</v>
@@ -30697,17 +30716,20 @@
         <v>11079</v>
       </c>
       <c r="O22" s="128">
+        <v>20</v>
+      </c>
+      <c r="P22" s="128">
         <v>933</v>
       </c>
-      <c r="P22" s="128"/>
-      <c r="R22" s="26">
+      <c r="Q22" s="128"/>
+      <c r="S22" s="26">
         <v>2025</v>
       </c>
-      <c r="S22" s="3">
+      <c r="T22" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="31" t="str">
         <f>Processes_BASE!B13</f>
         <v>IFMEAF-E</v>
@@ -30733,13 +30755,13 @@
       <c r="L23" s="26"/>
       <c r="M23" s="89"/>
       <c r="N23" s="89"/>
-      <c r="O23" s="26"/>
+      <c r="O23" s="89"/>
       <c r="P23" s="26"/>
-      <c r="Q23" s="94">
+      <c r="Q23" s="26"/>
+      <c r="R23" s="94">
         <f>EB_Exist!K23/EB_Exist!F22</f>
         <v>9.8455813953488391</v>
       </c>
-      <c r="R23" s="26"/>
       <c r="S23" s="26"/>
       <c r="T23" s="26"/>
       <c r="U23" s="26"/>
@@ -30747,8 +30769,9 @@
       <c r="W23" s="26"/>
       <c r="X23" s="26"/>
       <c r="Y23" s="26"/>
-    </row>
-    <row r="24" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z23" s="26"/>
+    </row>
+    <row r="24" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
       <c r="D24" s="26"/>
@@ -30763,11 +30786,10 @@
       <c r="J24" s="93"/>
       <c r="K24" s="93"/>
       <c r="L24" s="93"/>
-      <c r="Q24" s="130">
+      <c r="R24" s="130">
         <f>EB_Exist!K24/EB_Exist!F22</f>
         <v>3.2818604651162797</v>
       </c>
-      <c r="R24" s="26"/>
       <c r="S24" s="26"/>
       <c r="T24" s="26"/>
       <c r="U24" s="26"/>
@@ -30775,8 +30797,9 @@
       <c r="W24" s="26"/>
       <c r="X24" s="26"/>
       <c r="Y24" s="26"/>
-    </row>
-    <row r="25" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z24" s="26"/>
+    </row>
+    <row r="25" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
       <c r="D25" s="26"/>
@@ -30791,11 +30814,10 @@
       <c r="J25" s="93"/>
       <c r="K25" s="93"/>
       <c r="L25" s="93"/>
-      <c r="Q25" s="130">
+      <c r="R25" s="130">
         <f>EB_Exist!K25/EB_Exist!F22</f>
         <v>12.96</v>
       </c>
-      <c r="R25" s="26"/>
       <c r="S25" s="26"/>
       <c r="T25" s="26"/>
       <c r="U25" s="26"/>
@@ -30803,8 +30825,9 @@
       <c r="W25" s="26"/>
       <c r="X25" s="26"/>
       <c r="Y25" s="26"/>
-    </row>
-    <row r="26" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z25" s="26"/>
+    </row>
+    <row r="26" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E26" s="99"/>
       <c r="F26" s="98" t="str">
         <f>RES_Mn!O2</f>
@@ -30828,22 +30851,22 @@
       <c r="L26" s="93">
         <v>0</v>
       </c>
-      <c r="P26" s="89">
+      <c r="Q26" s="89">
         <f>EB_Exist!F26</f>
         <v>3225</v>
       </c>
-      <c r="Q26" s="26"/>
-      <c r="S26" s="26">
+      <c r="R26" s="26"/>
+      <c r="T26" s="26">
         <v>1</v>
       </c>
-      <c r="T26" s="26"/>
       <c r="U26" s="26"/>
       <c r="V26" s="26"/>
       <c r="W26" s="26"/>
       <c r="X26" s="26"/>
       <c r="Y26" s="26"/>
-    </row>
-    <row r="27" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="26"/>
+    </row>
+    <row r="27" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="31" t="str">
         <f>RES_Mn!M15</f>
         <v>IFMEAF-N</v>
@@ -30867,29 +30890,28 @@
       <c r="J27" s="93"/>
       <c r="K27" s="93"/>
       <c r="L27" s="93"/>
-      <c r="Q27" s="127">
-        <f>Q23/2</f>
+      <c r="R27" s="127">
+        <f>R23/2</f>
         <v>4.9227906976744196</v>
       </c>
-      <c r="S27" s="26"/>
       <c r="T27" s="26"/>
       <c r="U27" s="26"/>
       <c r="V27" s="26"/>
       <c r="W27" s="26"/>
       <c r="X27" s="26"/>
       <c r="Y27" s="26"/>
-    </row>
-    <row r="28" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z27" s="26"/>
+    </row>
+    <row r="28" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="99" t="str">
         <f>RES_Mn!E2</f>
         <v>INDCMU</v>
       </c>
       <c r="F28" s="98"/>
-      <c r="Q28" s="250">
-        <f>Q24</f>
+      <c r="R28" s="250">
+        <f>R24</f>
         <v>3.2818604651162797</v>
       </c>
-      <c r="R28" s="26"/>
       <c r="S28" s="26"/>
       <c r="T28" s="26"/>
       <c r="U28" s="26"/>
@@ -30897,18 +30919,18 @@
       <c r="W28" s="26"/>
       <c r="X28" s="26"/>
       <c r="Y28" s="26"/>
-    </row>
-    <row r="29" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z28" s="26"/>
+    </row>
+    <row r="29" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E29" s="99" t="str">
         <f>RES_Mn!F2</f>
         <v>IFAELC</v>
       </c>
       <c r="F29" s="26"/>
-      <c r="Q29" s="127">
+      <c r="R29" s="127">
         <f>EB_Exist!U55</f>
         <v>10.08</v>
       </c>
-      <c r="R29" s="26"/>
       <c r="S29" s="26"/>
       <c r="T29" s="26"/>
       <c r="U29" s="26"/>
@@ -30916,18 +30938,18 @@
       <c r="W29" s="26"/>
       <c r="X29" s="26"/>
       <c r="Y29" s="26"/>
-    </row>
-    <row r="30" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z29" s="26"/>
+    </row>
+    <row r="30" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E30" s="99" t="str">
         <f>RES_Mn!G2</f>
         <v>IFACHA</v>
       </c>
       <c r="F30" s="38"/>
-      <c r="Q30" s="127">
-        <f>Q27*1.1</f>
+      <c r="R30" s="127">
+        <f>R27*1.1</f>
         <v>5.415069767441862</v>
       </c>
-      <c r="R30" s="26"/>
       <c r="S30" s="26"/>
       <c r="T30" s="26"/>
       <c r="U30" s="26"/>
@@ -30935,8 +30957,9 @@
       <c r="W30" s="26"/>
       <c r="X30" s="26"/>
       <c r="Y30" s="26"/>
-    </row>
-    <row r="31" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z30" s="26"/>
+    </row>
+    <row r="31" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="99" t="str">
         <f>RES_Mn!O2</f>
         <v>IFAMN</v>
@@ -30948,18 +30971,21 @@
       <c r="N31" s="128">
         <v>10072</v>
       </c>
-      <c r="O31" s="128"/>
-      <c r="P31" s="128">
+      <c r="O31" s="128">
+        <v>20</v>
+      </c>
+      <c r="P31" s="128"/>
+      <c r="Q31" s="128">
         <v>2102</v>
       </c>
-      <c r="R31" s="26">
+      <c r="S31" s="26">
         <v>2025</v>
       </c>
-      <c r="S31" s="3">
+      <c r="T31" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:26" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="31" t="str">
         <f>RES_Mn!M22</f>
         <v>IFMEAFB-N</v>
@@ -30983,45 +31009,45 @@
       <c r="J32" s="93"/>
       <c r="K32" s="93"/>
       <c r="L32" s="93"/>
-      <c r="Q32" s="127">
-        <f>Q23*0.25</f>
+      <c r="R32" s="127">
+        <f>R23*0.25</f>
         <v>2.4613953488372098</v>
       </c>
     </row>
-    <row r="33" spans="5:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="5:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="99" t="str">
         <f>E28</f>
         <v>INDCMU</v>
       </c>
       <c r="F33" s="98"/>
-      <c r="Q33" s="250">
-        <f>Q24</f>
+      <c r="R33" s="250">
+        <f>R24</f>
         <v>3.2818604651162797</v>
       </c>
     </row>
-    <row r="34" spans="5:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="5:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="99" t="str">
         <f>E29</f>
         <v>IFAELC</v>
       </c>
       <c r="F34" s="26"/>
-      <c r="Q34" s="127">
-        <f>Q29</f>
+      <c r="R34" s="127">
+        <f>R29</f>
         <v>10.08</v>
       </c>
     </row>
-    <row r="35" spans="5:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="5:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="99" t="str">
         <f>E30</f>
         <v>IFACHA</v>
       </c>
       <c r="F35" s="38"/>
-      <c r="Q35" s="127">
-        <f>Q23*0.75*1.1</f>
+      <c r="R35" s="127">
+        <f>R23*0.75*1.1</f>
         <v>8.1226046511627938</v>
       </c>
     </row>
-    <row r="36" spans="5:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="5:20" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F36" s="99" t="str">
         <f>F31</f>
         <v>IFAMN</v>
@@ -31033,14 +31059,17 @@
       <c r="N36" s="128">
         <v>11079</v>
       </c>
-      <c r="O36" s="128"/>
-      <c r="P36" s="128">
+      <c r="O36" s="128">
+        <v>20</v>
+      </c>
+      <c r="P36" s="128"/>
+      <c r="Q36" s="128">
         <v>933</v>
       </c>
-      <c r="R36" s="26">
+      <c r="S36" s="26">
         <v>2025</v>
       </c>
-      <c r="S36" s="3">
+      <c r="T36" s="3">
         <v>1</v>
       </c>
     </row>
@@ -31307,7 +31336,7 @@
       <c r="D2" s="121" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="358" t="s">
+      <c r="E2" s="339" t="s">
         <v>628</v>
       </c>
       <c r="F2" s="121" t="s">
@@ -31364,7 +31393,7 @@
       <c r="D3" s="121" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="358" t="s">
+      <c r="E3" s="339" t="s">
         <v>629</v>
       </c>
       <c r="F3" s="121" t="s">
@@ -33964,7 +33993,7 @@
   </sheetPr>
   <dimension ref="C1:AE105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -34000,7 +34029,7 @@
       <c r="D2" s="279" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="359" t="s">
+      <c r="E2" s="340" t="s">
         <v>628</v>
       </c>
       <c r="F2" s="279" t="s">
@@ -34034,7 +34063,7 @@
       <c r="D3" s="279" t="s">
         <v>205</v>
       </c>
-      <c r="E3" s="359" t="s">
+      <c r="E3" s="340" t="s">
         <v>630</v>
       </c>
       <c r="F3" s="279" t="s">

</xml_diff>

<commit_message>
some edits to FA
Nothing major, some editing and cleaning
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-FA.xlsx
+++ b/vt_REGION1_IND-FA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CCBFCD-9832-4B51-BEA7-72A67B457255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E04B7321-3634-4CA7-9292-75C6725CF210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="818" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="818" firstSheet="1" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About and Log" sheetId="64" r:id="rId1"/>
@@ -939,7 +939,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389" uniqueCount="652">
   <si>
     <t>Comment</t>
   </si>
@@ -3121,9 +3121,6 @@
     <t>Energy and material use</t>
   </si>
   <si>
-    <t>LITERATURE</t>
-  </si>
-  <si>
     <t>On CHAR</t>
   </si>
   <si>
@@ -3167,6 +3164,69 @@
   </si>
   <si>
     <t>NCAP_TLIFE</t>
+  </si>
+  <si>
+    <t>https://www.engineeringnews.co.za/article/regulator-approves-eskom-tariff-discounts-for-ferrochrome-groups-2023-11-06</t>
+  </si>
+  <si>
+    <t>Regulator approves Eskom tariff discounts for ferrochrome groups</t>
+  </si>
+  <si>
+    <t>Glencore-Merafe Venture</t>
+  </si>
+  <si>
+    <t>Boshoek</t>
+  </si>
+  <si>
+    <t>Wonderkop</t>
+  </si>
+  <si>
+    <t>Lion</t>
+  </si>
+  <si>
+    <t>Lyndenburg</t>
+  </si>
+  <si>
+    <t>MVA</t>
+  </si>
+  <si>
+    <t>Samancore Chrome</t>
+  </si>
+  <si>
+    <t>baseload sales of'</t>
+  </si>
+  <si>
+    <t>TWh</t>
+  </si>
+  <si>
+    <t>Ferrometals</t>
+  </si>
+  <si>
+    <t>Middleburg Ferrochrome</t>
+  </si>
+  <si>
+    <t>Tubatse ferrochrome</t>
+  </si>
+  <si>
+    <t>Tubatse Alloy</t>
+  </si>
+  <si>
+    <t>TC Smelters</t>
+  </si>
+  <si>
+    <t>Dikwene Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LITERATURE </t>
+  </si>
+  <si>
+    <t>Comment:</t>
+  </si>
+  <si>
+    <t>From the article it's not clear that these are all the operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">or just the ones that got the tarriff approvals. </t>
   </si>
 </sst>
 </file>
@@ -3186,7 +3246,7 @@
     <numFmt numFmtId="172" formatCode="0.0"/>
     <numFmt numFmtId="173" formatCode="[$£-809]#,##0.000;[Red]&quot;-&quot;[$£-809]#,##0.000"/>
   </numFmts>
-  <fonts count="95" x14ac:knownFonts="1">
+  <fonts count="96" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -3823,6 +3883,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF212529"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="24">
@@ -4660,7 +4727,7 @@
     <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="360">
+  <cellXfs count="364">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5298,27 +5365,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="27" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="7" borderId="41" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="7" borderId="43" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="41" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="43" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5337,10 +5383,31 @@
     <xf numFmtId="166" fontId="60" fillId="0" borderId="49" xfId="23" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="50" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="60" fillId="0" borderId="49" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="7" borderId="41" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="7" borderId="43" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="44" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="41" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="43" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="68" fillId="11" borderId="2" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5355,6 +5422,10 @@
     <xf numFmtId="0" fontId="68" fillId="12" borderId="0" xfId="23" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="23" applyBorder="1"/>
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="23" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="23" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="78">
     <cellStyle name="20% - Accent5 2" xfId="60" xr:uid="{5E09AC11-EE5C-47C6-AC38-01F75E51F2D0}"/>
@@ -7688,15 +7759,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>429389</xdr:colOff>
-      <xdr:row>184</xdr:row>
-      <xdr:rowOff>154490</xdr:rowOff>
+      <xdr:colOff>584654</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>330428</xdr:colOff>
-      <xdr:row>204</xdr:row>
-      <xdr:rowOff>723</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>113134</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7726,8 +7797,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="17069564" y="9612815"/>
-          <a:ext cx="4596863" cy="3846732"/>
+          <a:off x="8428772" y="38660294"/>
+          <a:ext cx="5197581" cy="4409469"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7928,7 +7999,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>616827</xdr:colOff>
+      <xdr:colOff>291857</xdr:colOff>
       <xdr:row>315</xdr:row>
       <xdr:rowOff>123607</xdr:rowOff>
     </xdr:to>
@@ -22069,8 +22140,8 @@
   </sheetPr>
   <dimension ref="A1:AC174"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+    <sheetView topLeftCell="A114" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I165" sqref="I165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -22104,7 +22175,7 @@
       <c r="E2" s="309"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="343" t="s">
+      <c r="B3" s="351" t="s">
         <v>241</v>
       </c>
       <c r="C3" s="139" t="s">
@@ -22113,21 +22184,21 @@
       <c r="E3" s="310"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="343"/>
+      <c r="B4" s="351"/>
       <c r="C4" s="139" t="s">
         <v>243</v>
       </c>
       <c r="E4" s="310"/>
     </row>
     <row r="5" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="344"/>
+      <c r="B5" s="352"/>
       <c r="C5" s="141" t="s">
         <v>244</v>
       </c>
       <c r="E5" s="310"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="345" t="s">
+      <c r="B6" s="353" t="s">
         <v>245</v>
       </c>
       <c r="C6" s="142" t="s">
@@ -22136,21 +22207,21 @@
       <c r="E6" s="310"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="346"/>
+      <c r="B7" s="354"/>
       <c r="C7" s="142" t="s">
         <v>247</v>
       </c>
       <c r="E7" s="310"/>
     </row>
     <row r="8" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="347"/>
+      <c r="B8" s="355"/>
       <c r="C8" s="143" t="s">
         <v>248</v>
       </c>
       <c r="E8" s="310"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="345" t="s">
+      <c r="B9" s="353" t="s">
         <v>249</v>
       </c>
       <c r="C9" s="142" t="s">
@@ -22159,21 +22230,21 @@
       <c r="E9" s="310"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="346"/>
+      <c r="B10" s="354"/>
       <c r="C10" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E10" s="310"/>
     </row>
     <row r="11" spans="2:5" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="347"/>
+      <c r="B11" s="355"/>
       <c r="C11" s="143" t="s">
         <v>252</v>
       </c>
       <c r="E11" s="310"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="345" t="s">
+      <c r="B12" s="353" t="s">
         <v>253</v>
       </c>
       <c r="C12" s="142" t="s">
@@ -22182,14 +22253,14 @@
       <c r="E12" s="310"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="346"/>
+      <c r="B13" s="354"/>
       <c r="C13" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E13" s="310"/>
     </row>
     <row r="14" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="347"/>
+      <c r="B14" s="355"/>
       <c r="C14" s="143" t="s">
         <v>254</v>
       </c>
@@ -22296,10 +22367,10 @@
       <c r="B21" s="318" t="s">
         <v>269</v>
       </c>
-      <c r="C21" s="341">
+      <c r="C21" s="347">
         <v>1200</v>
       </c>
-      <c r="D21" s="348" t="s">
+      <c r="D21" s="341" t="s">
         <v>511</v>
       </c>
       <c r="E21" s="319" t="s">
@@ -22326,8 +22397,8 @@
       <c r="B22" s="320" t="s">
         <v>271</v>
       </c>
-      <c r="C22" s="342"/>
-      <c r="D22" s="349"/>
+      <c r="C22" s="348"/>
+      <c r="D22" s="342"/>
       <c r="E22" s="321"/>
       <c r="Q22" s="144">
         <v>4.9000000000000004</v>
@@ -22372,13 +22443,13 @@
       <c r="B24" s="318" t="s">
         <v>512</v>
       </c>
-      <c r="C24" s="341">
+      <c r="C24" s="347">
         <v>110</v>
       </c>
-      <c r="D24" s="350">
+      <c r="D24" s="343">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E24" s="352">
+      <c r="E24" s="345">
         <v>28.047042804386201</v>
       </c>
       <c r="H24" s="135">
@@ -22400,9 +22471,9 @@
       <c r="B25" s="320" t="s">
         <v>278</v>
       </c>
-      <c r="C25" s="342"/>
-      <c r="D25" s="351"/>
-      <c r="E25" s="353"/>
+      <c r="C25" s="348"/>
+      <c r="D25" s="344"/>
+      <c r="E25" s="346"/>
       <c r="Q25" s="144">
         <f>Q22/Q23</f>
         <v>13.611111111111112</v>
@@ -22436,13 +22507,13 @@
       <c r="B27" s="318" t="s">
         <v>282</v>
       </c>
-      <c r="C27" s="341">
+      <c r="C27" s="347">
         <v>267</v>
       </c>
-      <c r="D27" s="341">
+      <c r="D27" s="347">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E27" s="354">
+      <c r="E27" s="349">
         <v>26.809100000000001</v>
       </c>
       <c r="H27" s="135">
@@ -22481,9 +22552,9 @@
       <c r="B28" s="320" t="s">
         <v>286</v>
       </c>
-      <c r="C28" s="342"/>
-      <c r="D28" s="342"/>
-      <c r="E28" s="355"/>
+      <c r="C28" s="348"/>
+      <c r="D28" s="348"/>
+      <c r="E28" s="350"/>
     </row>
     <row r="29" spans="2:29" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="316" t="s">
@@ -24601,11 +24672,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B6:B8"/>
@@ -24613,6 +24679,11 @@
     <mergeCell ref="B12:B14"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="Q19" r:id="rId1" xr:uid="{8CFFA192-6679-4FBF-B0CE-9327F43C0D73}"/>
@@ -24951,10 +25022,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A13:V341"/>
+  <dimension ref="A13:AE341"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -24963,13 +25034,17 @@
     <col min="2" max="3" width="30.42578125" style="135" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="135" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="135" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="135" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="135" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="135"/>
     <col min="8" max="8" width="12.42578125" style="135" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" style="135" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="135" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" style="135" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="135"/>
+    <col min="12" max="14" width="9.140625" style="135"/>
+    <col min="15" max="15" width="15.5703125" style="135" customWidth="1"/>
+    <col min="16" max="25" width="9.140625" style="135"/>
+    <col min="26" max="26" width="15.42578125" style="135" customWidth="1"/>
+    <col min="27" max="16384" width="9.140625" style="135"/>
   </cols>
   <sheetData>
     <row r="13" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -24988,7 +25063,7 @@
       <c r="E14" s="309"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="343" t="s">
+      <c r="B15" s="351" t="s">
         <v>241</v>
       </c>
       <c r="C15" s="139" t="s">
@@ -24997,21 +25072,21 @@
       <c r="E15" s="310"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="343"/>
+      <c r="B16" s="351"/>
       <c r="C16" s="139" t="s">
         <v>243</v>
       </c>
       <c r="E16" s="310"/>
     </row>
     <row r="17" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="344"/>
+      <c r="B17" s="352"/>
       <c r="C17" s="141" t="s">
         <v>244</v>
       </c>
       <c r="E17" s="310"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="345" t="s">
+      <c r="B18" s="353" t="s">
         <v>245</v>
       </c>
       <c r="C18" s="142" t="s">
@@ -25020,21 +25095,21 @@
       <c r="E18" s="310"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="346"/>
+      <c r="B19" s="354"/>
       <c r="C19" s="142" t="s">
         <v>247</v>
       </c>
       <c r="E19" s="310"/>
     </row>
     <row r="20" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="347"/>
+      <c r="B20" s="355"/>
       <c r="C20" s="143" t="s">
         <v>248</v>
       </c>
       <c r="E20" s="310"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="345" t="s">
+      <c r="B21" s="353" t="s">
         <v>249</v>
       </c>
       <c r="C21" s="142" t="s">
@@ -25043,21 +25118,21 @@
       <c r="E21" s="310"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="346"/>
+      <c r="B22" s="354"/>
       <c r="C22" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E22" s="310"/>
     </row>
     <row r="23" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="347"/>
+      <c r="B23" s="355"/>
       <c r="C23" s="143" t="s">
         <v>252</v>
       </c>
       <c r="E23" s="310"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="345" t="s">
+      <c r="B24" s="353" t="s">
         <v>253</v>
       </c>
       <c r="C24" s="142" t="s">
@@ -25066,14 +25141,14 @@
       <c r="E24" s="310"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25" s="346"/>
+      <c r="B25" s="354"/>
       <c r="C25" s="142" t="s">
         <v>251</v>
       </c>
       <c r="E25" s="310"/>
     </row>
     <row r="26" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="347"/>
+      <c r="B26" s="355"/>
       <c r="C26" s="143" t="s">
         <v>254</v>
       </c>
@@ -25161,10 +25236,10 @@
       <c r="B33" s="318" t="s">
         <v>269</v>
       </c>
-      <c r="C33" s="341">
+      <c r="C33" s="347">
         <v>1200</v>
       </c>
-      <c r="D33" s="348" t="s">
+      <c r="D33" s="341" t="s">
         <v>511</v>
       </c>
       <c r="E33" s="319" t="s">
@@ -25189,8 +25264,8 @@
       <c r="B34" s="320" t="s">
         <v>271</v>
       </c>
-      <c r="C34" s="342"/>
-      <c r="D34" s="349"/>
+      <c r="C34" s="348"/>
+      <c r="D34" s="342"/>
       <c r="E34" s="321"/>
     </row>
     <row r="35" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25221,13 +25296,13 @@
       <c r="B36" s="318" t="s">
         <v>512</v>
       </c>
-      <c r="C36" s="341">
+      <c r="C36" s="347">
         <v>110</v>
       </c>
-      <c r="D36" s="350">
+      <c r="D36" s="343">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E36" s="352">
+      <c r="E36" s="345">
         <v>28.047042804386201</v>
       </c>
       <c r="H36" s="135">
@@ -25242,9 +25317,9 @@
       <c r="B37" s="320" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="342"/>
-      <c r="D37" s="351"/>
-      <c r="E37" s="353"/>
+      <c r="C37" s="348"/>
+      <c r="D37" s="344"/>
+      <c r="E37" s="346"/>
     </row>
     <row r="38" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="316" t="s">
@@ -25268,13 +25343,13 @@
       <c r="B39" s="318" t="s">
         <v>282</v>
       </c>
-      <c r="C39" s="341">
+      <c r="C39" s="347">
         <v>267</v>
       </c>
-      <c r="D39" s="341">
+      <c r="D39" s="347">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E39" s="354">
+      <c r="E39" s="349">
         <v>26.809100000000001</v>
       </c>
       <c r="H39" s="135">
@@ -25299,9 +25374,9 @@
       <c r="B40" s="320" t="s">
         <v>286</v>
       </c>
-      <c r="C40" s="342"/>
-      <c r="D40" s="342"/>
-      <c r="E40" s="355"/>
+      <c r="C40" s="348"/>
+      <c r="D40" s="348"/>
+      <c r="E40" s="350"/>
     </row>
     <row r="41" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="316" t="s">
@@ -25489,7 +25564,7 @@
     </row>
     <row r="55" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A55" s="186" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
@@ -25502,7 +25577,7 @@
         <v>546</v>
       </c>
       <c r="D58" s="338" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="E58" s="338">
         <v>2017</v>
@@ -25586,7 +25661,7 @@
         <v>0.8</v>
       </c>
       <c r="M61" s="135" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="26.25" x14ac:dyDescent="0.4">
@@ -25754,7 +25829,7 @@
         <v>327</v>
       </c>
       <c r="K81" s="158" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="82" spans="3:11" x14ac:dyDescent="0.25">
@@ -25780,7 +25855,7 @@
       <c r="I82" s="163"/>
       <c r="J82" s="163"/>
       <c r="K82" s="135" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="83" spans="3:11" x14ac:dyDescent="0.25">
@@ -26078,7 +26153,7 @@
     </row>
     <row r="99" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A99" s="332" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.25">
@@ -26177,7 +26252,7 @@
     </row>
     <row r="108" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A108" s="332" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.25">
@@ -26380,7 +26455,7 @@
     </row>
     <row r="119" spans="2:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="331" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C119" s="178"/>
     </row>
@@ -26424,7 +26499,7 @@
         <v>0.88420601428571455</v>
       </c>
       <c r="K122" s="181" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="123" spans="2:16" x14ac:dyDescent="0.25">
@@ -26796,17 +26871,17 @@
         <v>413</v>
       </c>
     </row>
-    <row r="180" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:31" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A180" s="196" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="183" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B183" s="149" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:31" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B184" s="136" t="s">
         <v>307</v>
       </c>
@@ -26822,18 +26897,63 @@
       <c r="L184" s="137"/>
       <c r="M184" s="137"/>
       <c r="N184" s="138"/>
-    </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S184" s="360" t="s">
+        <v>632</v>
+      </c>
+      <c r="T184" s="137"/>
+      <c r="U184" s="137"/>
+      <c r="V184" s="137"/>
+      <c r="W184" s="137"/>
+      <c r="X184" s="137"/>
+      <c r="Y184" s="137"/>
+      <c r="Z184" s="137"/>
+      <c r="AA184" s="137"/>
+      <c r="AB184" s="137"/>
+      <c r="AC184" s="137"/>
+      <c r="AD184" s="137"/>
+      <c r="AE184" s="138"/>
+    </row>
+    <row r="185" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B185" s="144"/>
       <c r="N185" s="140"/>
-    </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S185" s="144" t="s">
+        <v>631</v>
+      </c>
+      <c r="T185" s="361"/>
+      <c r="U185" s="361"/>
+      <c r="V185" s="361"/>
+      <c r="W185" s="361"/>
+      <c r="X185" s="361"/>
+      <c r="Y185" s="361"/>
+      <c r="Z185" s="361"/>
+      <c r="AA185" s="361"/>
+      <c r="AB185" s="361"/>
+      <c r="AC185" s="361"/>
+      <c r="AD185" s="361"/>
+      <c r="AE185" s="140"/>
+    </row>
+    <row r="186" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B186" s="162" t="s">
         <v>308</v>
       </c>
       <c r="N186" s="140"/>
-    </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S186" s="144"/>
+      <c r="T186" s="361"/>
+      <c r="U186" s="362" t="s">
+        <v>638</v>
+      </c>
+      <c r="V186" s="361"/>
+      <c r="W186" s="361"/>
+      <c r="X186" s="361"/>
+      <c r="Y186" s="361"/>
+      <c r="Z186" s="361"/>
+      <c r="AA186" s="361"/>
+      <c r="AB186" s="361"/>
+      <c r="AC186" s="361"/>
+      <c r="AD186" s="361"/>
+      <c r="AE186" s="140"/>
+    </row>
+    <row r="187" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B187" s="144">
         <v>4100</v>
       </c>
@@ -26841,24 +26961,93 @@
         <v>185</v>
       </c>
       <c r="N187" s="140"/>
-    </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S187" s="162" t="s">
+        <v>633</v>
+      </c>
+      <c r="T187" s="361"/>
+      <c r="U187" s="158">
+        <f>SUM(U188:U191)</f>
+        <v>880</v>
+      </c>
+      <c r="V187" s="361"/>
+      <c r="W187" s="361"/>
+      <c r="X187" s="361"/>
+      <c r="Y187" s="361"/>
+      <c r="Z187" s="361"/>
+      <c r="AA187" s="361"/>
+      <c r="AB187" s="361"/>
+      <c r="AC187" s="361"/>
+      <c r="AD187" s="361"/>
+      <c r="AE187" s="140"/>
+    </row>
+    <row r="188" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B188" s="144"/>
       <c r="N188" s="140"/>
-    </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S188" s="144"/>
+      <c r="T188" s="361" t="s">
+        <v>634</v>
+      </c>
+      <c r="U188" s="361">
+        <v>130</v>
+      </c>
+      <c r="V188" s="361"/>
+      <c r="W188" s="361"/>
+      <c r="X188" s="361"/>
+      <c r="Y188" s="361"/>
+      <c r="Z188" s="361"/>
+      <c r="AA188" s="361"/>
+      <c r="AB188" s="361"/>
+      <c r="AC188" s="361"/>
+      <c r="AD188" s="361"/>
+      <c r="AE188" s="140"/>
+    </row>
+    <row r="189" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B189" s="162" t="s">
         <v>311</v>
       </c>
       <c r="N189" s="140"/>
-    </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S189" s="144"/>
+      <c r="T189" s="361" t="s">
+        <v>635</v>
+      </c>
+      <c r="U189" s="361">
+        <v>310</v>
+      </c>
+      <c r="V189" s="361"/>
+      <c r="W189" s="361"/>
+      <c r="X189" s="361"/>
+      <c r="Y189" s="361"/>
+      <c r="Z189" s="361"/>
+      <c r="AA189" s="361"/>
+      <c r="AB189" s="361"/>
+      <c r="AC189" s="361"/>
+      <c r="AD189" s="361"/>
+      <c r="AE189" s="140"/>
+    </row>
+    <row r="190" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B190" s="144" t="s">
         <v>316</v>
       </c>
       <c r="N190" s="140"/>
-    </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S190" s="144"/>
+      <c r="T190" s="361" t="s">
+        <v>636</v>
+      </c>
+      <c r="U190" s="361">
+        <v>275</v>
+      </c>
+      <c r="V190" s="361"/>
+      <c r="W190" s="361"/>
+      <c r="X190" s="361"/>
+      <c r="Y190" s="361"/>
+      <c r="Z190" s="361"/>
+      <c r="AA190" s="361"/>
+      <c r="AB190" s="361"/>
+      <c r="AC190" s="361"/>
+      <c r="AD190" s="361"/>
+      <c r="AE190" s="140"/>
+    </row>
+    <row r="191" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B191" s="144">
         <v>4800</v>
       </c>
@@ -26866,30 +27055,120 @@
         <v>185</v>
       </c>
       <c r="N191" s="140"/>
-    </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="S191" s="144"/>
+      <c r="T191" s="361" t="s">
+        <v>637</v>
+      </c>
+      <c r="U191" s="361">
+        <v>165</v>
+      </c>
+      <c r="V191" s="361"/>
+      <c r="W191" s="361"/>
+      <c r="X191" s="361"/>
+      <c r="Y191" s="361"/>
+      <c r="Z191" s="361"/>
+      <c r="AA191" s="361"/>
+      <c r="AB191" s="361"/>
+      <c r="AC191" s="361"/>
+      <c r="AD191" s="361"/>
+      <c r="AE191" s="140"/>
+    </row>
+    <row r="192" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B192" s="144"/>
       <c r="N192" s="140"/>
-    </row>
-    <row r="193" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S192" s="144"/>
+      <c r="T192" s="361"/>
+      <c r="U192" s="361"/>
+      <c r="V192" s="361"/>
+      <c r="W192" s="361"/>
+      <c r="X192" s="361"/>
+      <c r="Y192" s="361"/>
+      <c r="Z192" s="361"/>
+      <c r="AA192" s="361"/>
+      <c r="AB192" s="361"/>
+      <c r="AC192" s="361"/>
+      <c r="AD192" s="361"/>
+      <c r="AE192" s="140"/>
+    </row>
+    <row r="193" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B193" s="162" t="s">
         <v>260</v>
       </c>
       <c r="N193" s="140"/>
-    </row>
-    <row r="194" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S193" s="162" t="s">
+        <v>639</v>
+      </c>
+      <c r="T193" s="361"/>
+      <c r="U193" s="362">
+        <f>SUM(U194:U199)</f>
+        <v>1363</v>
+      </c>
+      <c r="V193" s="361"/>
+      <c r="W193" s="363" t="s">
+        <v>640</v>
+      </c>
+      <c r="X193" s="361"/>
+      <c r="Y193" s="361">
+        <v>7.6</v>
+      </c>
+      <c r="Z193" s="361" t="s">
+        <v>641</v>
+      </c>
+      <c r="AA193" s="361"/>
+      <c r="AB193" s="361"/>
+      <c r="AC193" s="361"/>
+      <c r="AD193" s="361"/>
+      <c r="AE193" s="140"/>
+    </row>
+    <row r="194" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B194" s="144" t="s">
         <v>318</v>
       </c>
       <c r="N194" s="140"/>
-    </row>
-    <row r="195" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S194" s="144"/>
+      <c r="T194" s="361" t="s">
+        <v>642</v>
+      </c>
+      <c r="U194" s="361">
+        <v>270</v>
+      </c>
+      <c r="V194" s="361"/>
+      <c r="W194" s="361"/>
+      <c r="X194" s="361"/>
+      <c r="Y194" s="361"/>
+      <c r="Z194" s="361"/>
+      <c r="AA194" s="361"/>
+      <c r="AB194" s="361"/>
+      <c r="AC194" s="361"/>
+      <c r="AD194" s="361"/>
+      <c r="AE194" s="140"/>
+    </row>
+    <row r="195" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B195" s="144" t="s">
         <v>320</v>
       </c>
       <c r="N195" s="140"/>
-    </row>
-    <row r="196" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S195" s="144"/>
+      <c r="T195" s="361" t="s">
+        <v>643</v>
+      </c>
+      <c r="U195" s="361">
+        <v>286</v>
+      </c>
+      <c r="V195" s="361"/>
+      <c r="W195" s="361"/>
+      <c r="X195" s="361"/>
+      <c r="Y195" s="361"/>
+      <c r="Z195" s="197" t="s">
+        <v>649</v>
+      </c>
+      <c r="AA195" s="137"/>
+      <c r="AB195" s="137"/>
+      <c r="AC195" s="137"/>
+      <c r="AD195" s="137"/>
+      <c r="AE195" s="138"/>
+    </row>
+    <row r="196" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B196" s="144">
         <v>3500</v>
       </c>
@@ -26897,30 +27176,115 @@
         <v>185</v>
       </c>
       <c r="N196" s="140"/>
-    </row>
-    <row r="197" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S196" s="144"/>
+      <c r="T196" s="361" t="s">
+        <v>644</v>
+      </c>
+      <c r="U196" s="361">
+        <v>245</v>
+      </c>
+      <c r="V196" s="361"/>
+      <c r="W196" s="361"/>
+      <c r="X196" s="361"/>
+      <c r="Y196" s="361"/>
+      <c r="Z196" s="144" t="s">
+        <v>650</v>
+      </c>
+      <c r="AA196" s="361"/>
+      <c r="AB196" s="361"/>
+      <c r="AC196" s="361"/>
+      <c r="AD196" s="361"/>
+      <c r="AE196" s="140"/>
+    </row>
+    <row r="197" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B197" s="144"/>
       <c r="N197" s="140"/>
-    </row>
-    <row r="198" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S197" s="144"/>
+      <c r="T197" s="361" t="s">
+        <v>645</v>
+      </c>
+      <c r="U197" s="361">
+        <v>220</v>
+      </c>
+      <c r="V197" s="361"/>
+      <c r="W197" s="361"/>
+      <c r="X197" s="361"/>
+      <c r="Y197" s="361"/>
+      <c r="Z197" s="144" t="s">
+        <v>651</v>
+      </c>
+      <c r="AA197" s="361"/>
+      <c r="AB197" s="361"/>
+      <c r="AC197" s="361"/>
+      <c r="AD197" s="361"/>
+      <c r="AE197" s="140"/>
+    </row>
+    <row r="198" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B198" s="162" t="s">
         <v>319</v>
       </c>
       <c r="N198" s="140"/>
-    </row>
-    <row r="199" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S198" s="144"/>
+      <c r="T198" s="361" t="s">
+        <v>646</v>
+      </c>
+      <c r="U198" s="361">
+        <v>140</v>
+      </c>
+      <c r="V198" s="361"/>
+      <c r="W198" s="361"/>
+      <c r="X198" s="361"/>
+      <c r="Y198" s="361"/>
+      <c r="Z198" s="144"/>
+      <c r="AA198" s="361"/>
+      <c r="AB198" s="361"/>
+      <c r="AC198" s="361"/>
+      <c r="AD198" s="361"/>
+      <c r="AE198" s="140"/>
+    </row>
+    <row r="199" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B199" s="144" t="s">
         <v>323</v>
       </c>
       <c r="N199" s="140"/>
-    </row>
-    <row r="200" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S199" s="144"/>
+      <c r="T199" s="361" t="s">
+        <v>647</v>
+      </c>
+      <c r="U199" s="361">
+        <v>202</v>
+      </c>
+      <c r="V199" s="361"/>
+      <c r="W199" s="361"/>
+      <c r="X199" s="361"/>
+      <c r="Y199" s="361"/>
+      <c r="Z199" s="144"/>
+      <c r="AA199" s="361"/>
+      <c r="AB199" s="361"/>
+      <c r="AC199" s="361"/>
+      <c r="AD199" s="361"/>
+      <c r="AE199" s="140"/>
+    </row>
+    <row r="200" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B200" s="144" t="s">
         <v>324</v>
       </c>
       <c r="N200" s="140"/>
-    </row>
-    <row r="201" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S200" s="144"/>
+      <c r="T200" s="361"/>
+      <c r="U200" s="361"/>
+      <c r="V200" s="361"/>
+      <c r="W200" s="361"/>
+      <c r="X200" s="361"/>
+      <c r="Y200" s="361"/>
+      <c r="Z200" s="144"/>
+      <c r="AA200" s="361"/>
+      <c r="AB200" s="361"/>
+      <c r="AC200" s="361"/>
+      <c r="AD200" s="361"/>
+      <c r="AE200" s="140"/>
+    </row>
+    <row r="201" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B201" s="144">
         <v>2400</v>
       </c>
@@ -26928,24 +27292,50 @@
         <v>185</v>
       </c>
       <c r="N201" s="140"/>
-    </row>
-    <row r="202" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S201" s="144"/>
+      <c r="T201" s="361"/>
+      <c r="U201" s="361"/>
+      <c r="V201" s="361"/>
+      <c r="W201" s="361"/>
+      <c r="X201" s="361"/>
+      <c r="Y201" s="361"/>
+      <c r="Z201" s="144"/>
+      <c r="AA201" s="361"/>
+      <c r="AB201" s="361"/>
+      <c r="AC201" s="361"/>
+      <c r="AD201" s="361"/>
+      <c r="AE201" s="140"/>
+    </row>
+    <row r="202" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B202" s="144"/>
       <c r="N202" s="140"/>
-    </row>
-    <row r="203" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="S202" s="150"/>
+      <c r="T202" s="151"/>
+      <c r="U202" s="151"/>
+      <c r="V202" s="151"/>
+      <c r="W202" s="151"/>
+      <c r="X202" s="151"/>
+      <c r="Y202" s="151"/>
+      <c r="Z202" s="150"/>
+      <c r="AA202" s="151"/>
+      <c r="AB202" s="151"/>
+      <c r="AC202" s="151"/>
+      <c r="AD202" s="151"/>
+      <c r="AE202" s="152"/>
+    </row>
+    <row r="203" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B203" s="144"/>
       <c r="N203" s="140"/>
     </row>
-    <row r="204" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B204" s="144"/>
       <c r="N204" s="140"/>
     </row>
-    <row r="205" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B205" s="144"/>
       <c r="N205" s="140"/>
     </row>
-    <row r="206" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B206" s="150"/>
       <c r="C206" s="151"/>
       <c r="D206" s="151"/>
@@ -26960,7 +27350,7 @@
       <c r="M206" s="151"/>
       <c r="N206" s="152"/>
     </row>
-    <row r="208" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B208" s="135" t="s">
         <v>337</v>
       </c>
@@ -27263,7 +27653,7 @@
     </row>
     <row r="261" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B261" s="158" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="262" spans="2:14" x14ac:dyDescent="0.25">
@@ -27599,7 +27989,7 @@
     <row r="317" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B317" s="144"/>
       <c r="D317" s="330" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="N317" s="140"/>
     </row>
@@ -27811,18 +28201,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="D33:D34"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
     <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B273" r:id="rId1" xr:uid="{422A1BB5-B0D8-4A2F-BF63-C584298D04BA}"/>
@@ -30170,11 +30560,11 @@
   </sheetPr>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23:S26"/>
+      <selection pane="bottomRight" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -30359,7 +30749,7 @@
         <v>193</v>
       </c>
       <c r="O7" s="39" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="P7" s="92" t="str">
         <f>"ENV_ACT~"&amp;P5</f>
@@ -31337,7 +31727,7 @@
         <v>204</v>
       </c>
       <c r="E2" s="339" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F2" s="121" t="s">
         <v>202</v>
@@ -31394,7 +31784,7 @@
         <v>205</v>
       </c>
       <c r="E3" s="339" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F3" s="121" t="s">
         <v>203</v>
@@ -34030,7 +34420,7 @@
         <v>204</v>
       </c>
       <c r="E2" s="340" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F2" s="279" t="s">
         <v>202</v>
@@ -34064,7 +34454,7 @@
         <v>205</v>
       </c>
       <c r="E3" s="340" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F3" s="279" t="s">
         <v>203</v>
@@ -36314,7 +36704,7 @@
   <dimension ref="A1:AD78"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
DMD_PRJ bug fix + metals tweaks
DMD_PRJ for freight was pulling the incorrect driver. Have fixed this, but does need to be more automated in future.

Slight tweak to intensity values for FA. nothing major. Added a bit on why emissions factor seemed so high. it's correct though.
Slight change to electricity intensity for steel. It's really high, but it's the number from AMSA....
</commit_message>
<xml_diff>
--- a/vt_REGION1_IND-FA.xlsx
+++ b/vt_REGION1_IND-FA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA2C0278-8CE8-4812-8E0E-554FCAEA4B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FF4DB9-43DF-4282-8BE3-932B72B1F42E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="818" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="818" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About and Log" sheetId="64" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="CommData_BASE" sheetId="30" r:id="rId14"/>
     <sheet name="ANSv2-692-ProcData" sheetId="25" state="veryHidden" r:id="rId15"/>
     <sheet name="Chrome methodology" sheetId="70" r:id="rId16"/>
-    <sheet name="Sheet1" sheetId="71" r:id="rId17"/>
+    <sheet name="Emissions debate" sheetId="72" r:id="rId17"/>
     <sheet name="RES of chrome industry with EE" sheetId="65" r:id="rId18"/>
     <sheet name="ANSv2-692-ConstrData" sheetId="24" state="veryHidden" r:id="rId19"/>
     <sheet name="ANSv2-692-ITEMS" sheetId="10" state="veryHidden" r:id="rId20"/>
@@ -909,7 +909,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1219" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="667">
   <si>
     <t>Comment</t>
   </si>
@@ -3133,37 +3133,115 @@
     <t>assumption: drop Capacity gradually</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Indicator</t>
-  </si>
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>Subsector</t>
-  </si>
-  <si>
-    <t>TechDescription</t>
-  </si>
-  <si>
-    <t>Commodity Short Description</t>
-  </si>
-  <si>
-    <t>FlowOut</t>
-  </si>
-  <si>
-    <t>testChrome</t>
-  </si>
-  <si>
-    <t>FerroAlloys</t>
-  </si>
-  <si>
-    <t>FerroChrome Metal</t>
-  </si>
-  <si>
     <t>NCAP_BND~UP</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Ferrochromium produced</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>tCO2/tonne</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Ferromanganeses (7% C) produced</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Ferromanganeses (1% C) produced</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Ferrosilicon 65% Si produced</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Ferrosilicon 75% Si produced</t>
+  </si>
+  <si>
+    <t>Mass of CO2 per tonne Silicon metal produced</t>
+  </si>
+  <si>
+    <t>Amount of ferroalloy production - Ferrovanadium</t>
+  </si>
+  <si>
+    <t>Amount of ferroalloy production - Silicomanganese</t>
+  </si>
+  <si>
+    <t>Amount of ferroalloy production - Other ferroalloys</t>
+  </si>
+  <si>
+    <t>Mass of CH4 per tonne Ferrosilicon 65% Si produced</t>
+  </si>
+  <si>
+    <t>CH4</t>
+  </si>
+  <si>
+    <t>kg CH4/tonne</t>
+  </si>
+  <si>
+    <t>Mass of CH4 per tonne Silicon metal produced</t>
+  </si>
+  <si>
+    <t>Emissions inventory for SA.</t>
+  </si>
+  <si>
+    <t>Emissions factors from IPCC guidelines: Vol3 - metals industries</t>
+  </si>
+  <si>
+    <t>GJ/t chrome</t>
+  </si>
+  <si>
+    <t>Intensity in SATIM</t>
+  </si>
+  <si>
+    <t>In native units</t>
+  </si>
+  <si>
+    <t>IPPU emissions factors for reagents</t>
+  </si>
+  <si>
+    <t>t CO2/tonne reducing agent</t>
+  </si>
+  <si>
+    <t>tonnes of reducing agent / tonne of chrome</t>
+  </si>
+  <si>
+    <t>Inferred IPPU emissions factor for chrome</t>
+  </si>
+  <si>
+    <t>CO2/tonne of chrome</t>
+  </si>
+  <si>
+    <t>Emissions of CO2 based on mass:</t>
+  </si>
+  <si>
+    <t>Carbon content %</t>
+  </si>
+  <si>
+    <t>t Carbon per tonne of reducing agent</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>mass in kg</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>total Carbon</t>
+  </si>
+  <si>
+    <t>inferreed CO2</t>
+  </si>
+  <si>
+    <t>Emissions factor for ferrochrome:</t>
+  </si>
+  <si>
+    <t>Using IPPU emissions factors</t>
+  </si>
+  <si>
+    <t>Using mass balance of coal and coke</t>
   </si>
 </sst>
 </file>
@@ -4663,7 +4741,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="96" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="343">
+  <cellXfs count="349">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5269,43 +5347,6 @@
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="22" quotePrefix="1"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="53" fillId="0" borderId="0" xfId="77" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="68" fillId="10" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="10" borderId="3" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="10" borderId="31" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="68" fillId="11" borderId="0" xfId="22" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="60" fillId="0" borderId="28" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="60" fillId="0" borderId="29" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="60" fillId="0" borderId="50" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="60" fillId="0" borderId="49" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="50" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="49" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="75" fillId="0" borderId="28" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5327,6 +5368,49 @@
     <xf numFmtId="0" fontId="55" fillId="0" borderId="43" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="28" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="29" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="10" borderId="2" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="10" borderId="3" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="10" borderId="31" xfId="22" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="68" fillId="11" borderId="0" xfId="22" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="60" fillId="0" borderId="28" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="60" fillId="0" borderId="29" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="60" fillId="0" borderId="50" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="60" fillId="0" borderId="49" xfId="22" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="50" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="49" xfId="22" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="18" applyFont="1"/>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="78">
     <cellStyle name="20% - Accent5 2" xfId="59" xr:uid="{5E09AC11-EE5C-47C6-AC38-01F75E51F2D0}"/>
@@ -6662,11 +6746,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>960120</xdr:colOff>
-      <xdr:row>247</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>511885</xdr:colOff>
+      <xdr:row>246</xdr:row>
+      <xdr:rowOff>269635</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="4939240" cy="4248150"/>
+    <xdr:ext cx="5147085" cy="4426914"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
@@ -6695,8 +6779,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="8808720" y="50364390"/>
-          <a:ext cx="4939240" cy="4248150"/>
+          <a:off x="8356003" y="52253723"/>
+          <a:ext cx="5147085" cy="4426914"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6718,11 +6802,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>340995</xdr:colOff>
-      <xdr:row>270</xdr:row>
-      <xdr:rowOff>79215</xdr:rowOff>
+      <xdr:colOff>217730</xdr:colOff>
+      <xdr:row>268</xdr:row>
+      <xdr:rowOff>774</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5335905" cy="4483929"/>
+    <xdr:ext cx="6203240" cy="5212778"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
@@ -6751,8 +6835,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="16981170" y="18938715"/>
-          <a:ext cx="5335905" cy="4483929"/>
+          <a:off x="8061848" y="56736156"/>
+          <a:ext cx="6203240" cy="5212778"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7314,6 +7398,189 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>95684</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B3E1C2-A95D-9E28-0A88-51B8CB75AA4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="4533901"/>
+          <a:ext cx="6219825" cy="3010333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>52784</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253E4817-7EBD-EB37-58F2-31A8C4B840C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257301" y="7677150"/>
+          <a:ext cx="6191249" cy="3224609"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E16936E8-1D11-15F8-1A31-FD3F2F44FD86}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1295400" y="76200"/>
+          <a:ext cx="7239000" cy="1438275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100"/>
+            <a:t>The emissions factor in the inventory seemed very high</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100" baseline="0"/>
+            <a:t> (3.22 per tonne of ferrochrome) compared to the IPCC guidelines, which has a generic emissions factor of 1.6 as per table 4.5. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-ZA" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100" baseline="0"/>
+            <a:t>Having then used the emissions factor for the reducing agents from table 4.6 + the reducing agent inputs intensity as per the literature review then the emissions factors come out to be around 2.9 or so, so 3.22 seems to be ok to use. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-ZA" sz="1100" b="1" baseline="0"/>
+            <a:t>It's not clear why the emissions factor for ferrochrome in table 4.5 is then so low. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-ZA" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -7358,7 +7625,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -8451,7 +8718,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -9000,7 +9267,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -10365,7 +10632,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -11458,7 +11725,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -12823,7 +13090,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -14154,1099 +14421,6 @@
         <a:xfrm>
           <a:off x="19050" y="542925"/>
           <a:ext cx="819150" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61442" name="cmdCheckTIDTradeSheet" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61442"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000002F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61443" name="cmdSpecifyParameter" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61443"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000003F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61444" name="cmdSpecifyArg1" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61444"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000004F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61445" name="cmdSpecifyArg2" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61445"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000005F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61446" name="cmdSpecifyArg3" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61446"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000006F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61447" name="cmdSpecifyArg4" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61447"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000007F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61448" name="cmdSpecifyArg5" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61448"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000008F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="61449" name="cmdSpecifyArg6" hidden="1">
-          <a:extLst>
-            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61449"/>
-            </a:ext>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000009F00000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>828675</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="cmdCheckTIDTradeSheet">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE67A060-C88F-4951-BD9F-BF84866539AE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="9525" y="285750"/>
-          <a:ext cx="819150" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="cmdSpecifyParameter">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E85F9BC-6A63-4102-922B-5F718AB72A65}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1590675" y="495300"/>
-          <a:ext cx="819150" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="cmdSpecifyArg1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BAF8459-9485-4533-AC41-674A41E17EB7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2390775" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="cmdSpecifyArg2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70078D9D-8226-47C9-A210-B2107EF225DF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3019425" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="cmdSpecifyArg3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0AEA346-E5D7-4CED-A527-CDF07EE38434}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3638550" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="cmdSpecifyArg4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3216FB0F-236E-4EC7-8C81-2430BF5226E2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4248150" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="cmdSpecifyArg5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820EFD9B-E365-4EF1-A5FC-29BA8B47774E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="4857750" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="cmdSpecifyArg6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACAC6C77-992F-42FD-A0C5-587D0DF77CF4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5467350" y="495300"/>
-          <a:ext cx="619125" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15727,6 +14901,1099 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61442" name="cmdCheckTIDTradeSheet" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61442"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000002F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61443" name="cmdSpecifyParameter" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61443"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000003F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61444" name="cmdSpecifyArg1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61444"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000004F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61445" name="cmdSpecifyArg2" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61445"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000005F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61446" name="cmdSpecifyArg3" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61446"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000006F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61447" name="cmdSpecifyArg4" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61447"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000007F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61448" name="cmdSpecifyArg5" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61448"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000008F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61449" name="cmdSpecifyArg6" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s61449"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-1400-000009F00000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>828675</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="cmdCheckTIDTradeSheet">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE67A060-C88F-4951-BD9F-BF84866539AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9525" y="285750"/>
+          <a:ext cx="819150" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="cmdSpecifyParameter">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E85F9BC-6A63-4102-922B-5F718AB72A65}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1590675" y="495300"/>
+          <a:ext cx="819150" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="cmdSpecifyArg1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BAF8459-9485-4533-AC41-674A41E17EB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2390775" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="cmdSpecifyArg2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70078D9D-8226-47C9-A210-B2107EF225DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3019425" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="cmdSpecifyArg3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0AEA346-E5D7-4CED-A527-CDF07EE38434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3638550" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="cmdSpecifyArg4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3216FB0F-236E-4EC7-8C81-2430BF5226E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4248150" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="cmdSpecifyArg5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820EFD9B-E365-4EF1-A5FC-29BA8B47774E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4857750" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="cmdSpecifyArg6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACAC6C77-992F-42FD-A0C5-587D0DF77CF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5467350" y="495300"/>
+          <a:ext cx="619125" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing21.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
@@ -19790,6 +20057,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20945,8 +21216,8 @@
   </sheetPr>
   <dimension ref="A6:AG387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T169" sqref="T169"/>
+    <sheetView topLeftCell="A123" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P72" sqref="P72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -20995,7 +21266,7 @@
       <c r="E9" s="287"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="338" t="s">
+      <c r="B10" s="325" t="s">
         <v>221</v>
       </c>
       <c r="C10" s="126" t="s">
@@ -21004,21 +21275,21 @@
       <c r="E10" s="288"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="338"/>
+      <c r="B11" s="325"/>
       <c r="C11" s="126" t="s">
         <v>223</v>
       </c>
       <c r="E11" s="288"/>
     </row>
     <row r="12" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="339"/>
+      <c r="B12" s="326"/>
       <c r="C12" s="128" t="s">
         <v>224</v>
       </c>
       <c r="E12" s="288"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="340" t="s">
+      <c r="B13" s="327" t="s">
         <v>225</v>
       </c>
       <c r="C13" s="129" t="s">
@@ -21027,21 +21298,21 @@
       <c r="E13" s="288"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="341"/>
+      <c r="B14" s="328"/>
       <c r="C14" s="129" t="s">
         <v>227</v>
       </c>
       <c r="E14" s="288"/>
     </row>
     <row r="15" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="342"/>
+      <c r="B15" s="329"/>
       <c r="C15" s="130" t="s">
         <v>228</v>
       </c>
       <c r="E15" s="288"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="340" t="s">
+      <c r="B16" s="327" t="s">
         <v>229</v>
       </c>
       <c r="C16" s="129" t="s">
@@ -21050,21 +21321,21 @@
       <c r="E16" s="288"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="341"/>
+      <c r="B17" s="328"/>
       <c r="C17" s="129" t="s">
         <v>231</v>
       </c>
       <c r="E17" s="288"/>
     </row>
     <row r="18" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="342"/>
+      <c r="B18" s="329"/>
       <c r="C18" s="130" t="s">
         <v>232</v>
       </c>
       <c r="E18" s="288"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="340" t="s">
+      <c r="B19" s="327" t="s">
         <v>233</v>
       </c>
       <c r="C19" s="129" t="s">
@@ -21073,14 +21344,14 @@
       <c r="E19" s="288"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="341"/>
+      <c r="B20" s="328"/>
       <c r="C20" s="129" t="s">
         <v>231</v>
       </c>
       <c r="E20" s="288"/>
     </row>
     <row r="21" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="342"/>
+      <c r="B21" s="329"/>
       <c r="C21" s="130" t="s">
         <v>234</v>
       </c>
@@ -21168,10 +21439,10 @@
       <c r="B28" s="296" t="s">
         <v>248</v>
       </c>
-      <c r="C28" s="328">
+      <c r="C28" s="330">
         <v>1200</v>
       </c>
-      <c r="D28" s="336" t="s">
+      <c r="D28" s="323" t="s">
         <v>469</v>
       </c>
       <c r="E28" s="297" t="s">
@@ -21196,8 +21467,8 @@
       <c r="B29" s="298" t="s">
         <v>250</v>
       </c>
-      <c r="C29" s="329"/>
-      <c r="D29" s="337"/>
+      <c r="C29" s="331"/>
+      <c r="D29" s="324"/>
       <c r="E29" s="299"/>
     </row>
     <row r="30" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -21228,13 +21499,13 @@
       <c r="B31" s="296" t="s">
         <v>470</v>
       </c>
-      <c r="C31" s="328">
+      <c r="C31" s="330">
         <v>110</v>
       </c>
-      <c r="D31" s="330">
+      <c r="D31" s="336">
         <v>-26.1357162831553</v>
       </c>
-      <c r="E31" s="332">
+      <c r="E31" s="338">
         <v>28.047042804386201</v>
       </c>
       <c r="H31" s="122">
@@ -21249,9 +21520,9 @@
       <c r="B32" s="298" t="s">
         <v>257</v>
       </c>
-      <c r="C32" s="329"/>
-      <c r="D32" s="331"/>
-      <c r="E32" s="333"/>
+      <c r="C32" s="331"/>
+      <c r="D32" s="337"/>
+      <c r="E32" s="339"/>
     </row>
     <row r="33" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="294" t="s">
@@ -21275,13 +21546,13 @@
       <c r="B34" s="296" t="s">
         <v>261</v>
       </c>
-      <c r="C34" s="328">
+      <c r="C34" s="330">
         <v>267</v>
       </c>
-      <c r="D34" s="328">
+      <c r="D34" s="330">
         <v>-26.903199999999998</v>
       </c>
-      <c r="E34" s="334">
+      <c r="E34" s="340">
         <v>26.809100000000001</v>
       </c>
       <c r="H34" s="122">
@@ -21306,9 +21577,9 @@
       <c r="B35" s="298" t="s">
         <v>265</v>
       </c>
-      <c r="C35" s="329"/>
-      <c r="D35" s="329"/>
-      <c r="E35" s="335"/>
+      <c r="C35" s="331"/>
+      <c r="D35" s="331"/>
+      <c r="E35" s="341"/>
     </row>
     <row r="36" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="294" t="s">
@@ -22500,7 +22771,7 @@
         <v>5.1583999999999998E-2</v>
       </c>
       <c r="H121" s="160">
-        <f t="shared" si="4"/>
+        <f>H$112*H83</f>
         <v>1.4975999999999998E-2</v>
       </c>
       <c r="I121" s="172">
@@ -22511,7 +22782,7 @@
         <v>272</v>
       </c>
       <c r="P121" s="122">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
@@ -22523,7 +22794,7 @@
         <v>0.23946300000000001</v>
       </c>
       <c r="G122" s="160">
-        <f t="shared" si="4"/>
+        <f>G$112*G84</f>
         <v>0.59321599999999997</v>
       </c>
       <c r="H122" s="160">
@@ -22593,7 +22864,7 @@
         <v>272</v>
       </c>
       <c r="P124" s="122">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="126" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
@@ -22620,7 +22891,7 @@
       </c>
       <c r="F128" s="162">
         <f>(I121*P121+I124*P124)/$I$112</f>
-        <v>4.0813818503582935</v>
+        <v>3.9494607908555515</v>
       </c>
       <c r="G128" s="122" t="s">
         <v>335</v>
@@ -22693,7 +22964,7 @@
       </c>
       <c r="P142" s="122">
         <f>H158/D158</f>
-        <v>0.67809159724869195</v>
+        <v>0.68159466044380879</v>
       </c>
     </row>
     <row r="143" spans="2:16" x14ac:dyDescent="0.25">
@@ -22864,7 +23135,7 @@
       </c>
       <c r="D155" s="160">
         <f>F128</f>
-        <v>4.0813818503582935</v>
+        <v>3.9494607908555515</v>
       </c>
       <c r="E155" s="160"/>
       <c r="F155" s="122" t="s">
@@ -22981,7 +23252,7 @@
       </c>
       <c r="D158" s="172">
         <f>SUMPRODUCT(D155:D157,Q155:Q157)</f>
-        <v>22.074495629696251</v>
+        <v>21.961043518523894</v>
       </c>
       <c r="E158" s="172"/>
       <c r="F158" s="145"/>
@@ -23146,7 +23417,7 @@
         <v>596</v>
       </c>
       <c r="M169" s="316" t="s">
-        <v>640</v>
+        <v>630</v>
       </c>
     </row>
     <row r="170" spans="1:22" x14ac:dyDescent="0.25">
@@ -23174,7 +23445,7 @@
       <c r="E171" s="90"/>
       <c r="F171" s="162">
         <f>D155</f>
-        <v>4.0813818503582935</v>
+        <v>3.9494607908555515</v>
       </c>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.25">
@@ -23234,7 +23505,7 @@
       <c r="E175" s="90"/>
       <c r="F175" s="162">
         <f>F171</f>
-        <v>4.0813818503582935</v>
+        <v>3.9494607908555515</v>
       </c>
       <c r="H175" s="148"/>
     </row>
@@ -23435,7 +23706,7 @@
       </c>
       <c r="L186" s="168">
         <f>L181*(J158-J157)/D158</f>
-        <v>1347.4799123919686</v>
+        <v>1354.4410770877294</v>
       </c>
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.25">
@@ -24396,15 +24667,15 @@
         <v>410</v>
       </c>
       <c r="T246" s="182"/>
-      <c r="U246" s="324" t="s">
+      <c r="U246" s="332" t="s">
         <v>411</v>
       </c>
-      <c r="V246" s="325"/>
-      <c r="W246" s="326" t="s">
+      <c r="V246" s="333"/>
+      <c r="W246" s="334" t="s">
         <v>412</v>
       </c>
-      <c r="X246" s="326"/>
-      <c r="Y246" s="326"/>
+      <c r="X246" s="334"/>
+      <c r="Y246" s="334"/>
       <c r="AB246" s="127"/>
     </row>
     <row r="247" spans="2:28" ht="28.5" x14ac:dyDescent="0.25">
@@ -24422,10 +24693,10 @@
       <c r="V247" s="187" t="s">
         <v>414</v>
       </c>
-      <c r="W247" s="327" t="s">
+      <c r="W247" s="335" t="s">
         <v>415</v>
       </c>
-      <c r="X247" s="327"/>
+      <c r="X247" s="335"/>
       <c r="Y247" s="188" t="s">
         <v>414</v>
       </c>
@@ -25633,12 +25904,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="C28:C29"/>
     <mergeCell ref="U246:V246"/>
     <mergeCell ref="W246:Y246"/>
     <mergeCell ref="W247:X247"/>
@@ -25648,6 +25913,12 @@
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="D34:D35"/>
     <mergeCell ref="E34:E35"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B312" r:id="rId1" xr:uid="{422A1BB5-B0D8-4A2F-BF63-C584298D04BA}"/>
@@ -25663,735 +25934,523 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FDA67A-800B-417B-BC35-8361CBF14557}">
-  <dimension ref="H14:AH31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C60741-6B9A-4F50-A71D-2E9A74A53075}">
+  <dimension ref="C12:Y81"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="12" max="12" width="34" customWidth="1"/>
-    <col min="15" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="14" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="N14" t="s">
-        <v>630</v>
-      </c>
-      <c r="O14" t="s">
-        <v>630</v>
-      </c>
-      <c r="P14" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>630</v>
-      </c>
-      <c r="R14" t="s">
-        <v>630</v>
-      </c>
-      <c r="S14" t="s">
-        <v>630</v>
-      </c>
-      <c r="T14" t="s">
-        <v>630</v>
-      </c>
-      <c r="U14" t="s">
-        <v>630</v>
-      </c>
-      <c r="V14" t="s">
-        <v>630</v>
-      </c>
-      <c r="W14" t="s">
-        <v>630</v>
-      </c>
-      <c r="X14" t="s">
-        <v>630</v>
-      </c>
-      <c r="Y14" t="s">
-        <v>630</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AG14" t="s">
-        <v>630</v>
-      </c>
-      <c r="AH14" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="15" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H15" t="s">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="342" t="s">
+        <v>646</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="67"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="65"/>
+      <c r="D13" s="343"/>
+      <c r="E13" s="343"/>
+      <c r="F13" s="344">
+        <v>2017</v>
+      </c>
+      <c r="G13" s="344">
+        <v>2020</v>
+      </c>
+      <c r="H13" s="225"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="65" t="s">
         <v>631</v>
       </c>
-      <c r="I15" t="s">
+      <c r="D14" s="343" t="s">
         <v>632</v>
       </c>
-      <c r="J15" t="s">
+      <c r="E14" s="343" t="s">
         <v>633</v>
       </c>
-      <c r="K15" t="s">
-        <v>631</v>
-      </c>
-      <c r="L15" t="s">
+      <c r="F14" s="343">
+        <v>3.2245200000000001</v>
+      </c>
+      <c r="G14" s="343">
+        <v>3.2245200000000001</v>
+      </c>
+      <c r="H14" s="225"/>
+      <c r="J14" s="62"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="65" t="s">
         <v>634</v>
       </c>
-      <c r="M15" t="s">
+      <c r="D15" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E15" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F15" s="343">
+        <v>1.3</v>
+      </c>
+      <c r="G15" s="343">
+        <v>1.3</v>
+      </c>
+      <c r="H15" s="225"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="65" t="s">
         <v>635</v>
       </c>
-      <c r="N15">
-        <v>2019</v>
-      </c>
-      <c r="O15">
-        <v>2020</v>
-      </c>
-      <c r="P15">
-        <v>2021</v>
-      </c>
-      <c r="Q15">
-        <v>2022</v>
-      </c>
-      <c r="R15">
-        <v>2023</v>
-      </c>
-      <c r="S15">
-        <v>2024</v>
-      </c>
-      <c r="T15">
-        <v>2025</v>
-      </c>
-      <c r="U15">
-        <v>2026</v>
-      </c>
-      <c r="V15">
-        <v>2027</v>
-      </c>
-      <c r="W15">
-        <v>2028</v>
-      </c>
-      <c r="X15">
-        <v>2029</v>
-      </c>
-      <c r="Y15">
-        <v>2030</v>
-      </c>
-      <c r="Z15">
-        <v>2031</v>
-      </c>
-      <c r="AA15">
-        <v>2032</v>
-      </c>
-      <c r="AB15">
-        <v>2033</v>
-      </c>
-      <c r="AC15">
-        <v>2034</v>
-      </c>
-      <c r="AD15">
-        <v>2035</v>
-      </c>
-      <c r="AE15">
-        <v>2036</v>
-      </c>
-      <c r="AF15">
-        <v>2037</v>
-      </c>
-      <c r="AG15">
-        <v>2038</v>
-      </c>
-      <c r="AH15">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="16" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H16" t="s">
+      <c r="D16" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E16" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F16" s="343">
+        <v>1.5</v>
+      </c>
+      <c r="G16" s="343">
+        <v>1.5</v>
+      </c>
+      <c r="H16" s="225"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C17" s="65" t="s">
         <v>636</v>
       </c>
-      <c r="I16" t="s">
+      <c r="D17" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E17" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F17" s="343">
+        <v>3.6</v>
+      </c>
+      <c r="G17" s="343">
+        <v>3.6</v>
+      </c>
+      <c r="H17" s="225"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C18" s="65" t="s">
         <v>637</v>
       </c>
-      <c r="J16" t="s">
+      <c r="D18" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E18" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F18" s="343">
+        <v>4</v>
+      </c>
+      <c r="G18" s="343">
+        <v>4</v>
+      </c>
+      <c r="H18" s="225"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="65" t="s">
         <v>638</v>
       </c>
-      <c r="K16" t="s">
-        <v>636</v>
-      </c>
-      <c r="L16" t="s">
-        <v>605</v>
-      </c>
-      <c r="M16" t="s">
+      <c r="D19" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E19" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F19" s="343">
+        <v>5</v>
+      </c>
+      <c r="G19" s="343">
+        <v>5</v>
+      </c>
+      <c r="H19" s="225"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="65" t="s">
         <v>639</v>
       </c>
-      <c r="N16" s="323">
-        <v>3410</v>
-      </c>
-      <c r="O16" s="323">
-        <v>3097</v>
-      </c>
-      <c r="P16" s="323">
-        <v>3379</v>
-      </c>
-      <c r="Q16" s="323">
-        <v>3352</v>
-      </c>
-      <c r="R16" s="323">
-        <v>3356</v>
-      </c>
-      <c r="S16" s="323">
-        <v>3377</v>
-      </c>
-      <c r="T16" s="323">
-        <v>3402</v>
-      </c>
-      <c r="U16" s="323">
-        <v>3508</v>
-      </c>
-      <c r="V16" s="323">
-        <v>3601</v>
-      </c>
-      <c r="W16" s="323">
-        <v>3801</v>
-      </c>
-      <c r="X16" s="323">
-        <v>3953</v>
-      </c>
-      <c r="Y16" s="323">
-        <v>2434</v>
-      </c>
-      <c r="Z16" s="323">
-        <v>2194</v>
-      </c>
-      <c r="AA16" s="323">
-        <v>2197</v>
-      </c>
-      <c r="AB16" s="323">
-        <v>2315</v>
-      </c>
-      <c r="AC16" s="323">
-        <v>2457</v>
-      </c>
-      <c r="AD16" s="323">
-        <v>1234</v>
-      </c>
-      <c r="AE16">
-        <v>994</v>
-      </c>
-      <c r="AF16">
-        <v>754</v>
-      </c>
-      <c r="AG16">
-        <v>514</v>
-      </c>
-      <c r="AH16">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="17" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H17" t="s">
-        <v>214</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="D20" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E20" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F20" s="343"/>
+      <c r="G20" s="343"/>
+      <c r="H20" s="225"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="65" t="s">
+        <v>640</v>
+      </c>
+      <c r="D21" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E21" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F21" s="343">
+        <v>1.4</v>
+      </c>
+      <c r="G21" s="343">
+        <v>1.4</v>
+      </c>
+      <c r="H21" s="225"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C22" s="65" t="s">
+        <v>641</v>
+      </c>
+      <c r="D22" s="343" t="s">
+        <v>632</v>
+      </c>
+      <c r="E22" s="343" t="s">
+        <v>633</v>
+      </c>
+      <c r="F22" s="343"/>
+      <c r="G22" s="343"/>
+      <c r="H22" s="225"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C23" s="65" t="s">
+        <v>642</v>
+      </c>
+      <c r="D23" s="343" t="s">
+        <v>643</v>
+      </c>
+      <c r="E23" s="343" t="s">
+        <v>644</v>
+      </c>
+      <c r="F23" s="343">
+        <v>1</v>
+      </c>
+      <c r="G23" s="343">
+        <v>1</v>
+      </c>
+      <c r="H23" s="225"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C24" s="65" t="s">
         <v>637</v>
       </c>
-      <c r="J17" t="s">
-        <v>638</v>
-      </c>
-      <c r="K17" t="s">
-        <v>214</v>
-      </c>
-      <c r="L17" t="s">
-        <v>605</v>
-      </c>
-      <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="O17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="P17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="Q17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="R17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="S17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="T17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="U17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="V17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="W17" s="323">
-        <v>4857</v>
-      </c>
-      <c r="X17" s="323">
-        <v>4457</v>
-      </c>
-      <c r="Y17" s="323">
-        <v>4057</v>
-      </c>
-      <c r="Z17" s="323">
-        <v>3657</v>
-      </c>
-      <c r="AA17" s="323">
-        <v>3257</v>
-      </c>
-      <c r="AB17" s="323">
-        <v>2857</v>
-      </c>
-      <c r="AC17" s="323">
-        <v>2457</v>
-      </c>
-      <c r="AD17" s="323">
-        <v>2057</v>
-      </c>
-      <c r="AE17" s="323">
-        <v>1657</v>
-      </c>
-      <c r="AF17" s="323">
-        <v>1257</v>
-      </c>
-      <c r="AG17">
-        <v>857</v>
-      </c>
-      <c r="AH17">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="22" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="N22" s="227">
-        <f>N16/N17</f>
-        <v>0.7020794729256743</v>
-      </c>
-      <c r="O22" s="227">
-        <f>O16/O17</f>
-        <v>0.6376364010706197</v>
-      </c>
-      <c r="P22" s="227">
-        <f t="shared" ref="P22:AH22" si="0">P16/P17</f>
-        <v>0.69569693226271356</v>
-      </c>
-      <c r="Q22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.69013794523368333</v>
-      </c>
-      <c r="R22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.69096149886761371</v>
-      </c>
-      <c r="S22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.69528515544574843</v>
-      </c>
-      <c r="T22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.70043236565781342</v>
-      </c>
-      <c r="U22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.72225653695696934</v>
-      </c>
-      <c r="V22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.74140415894585132</v>
-      </c>
-      <c r="W22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.7825818406423718</v>
-      </c>
-      <c r="X22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.88691945254655602</v>
-      </c>
-      <c r="Y22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.59995070248952431</v>
-      </c>
-      <c r="Z22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.59994531036368604</v>
-      </c>
-      <c r="AA22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.67454712926005522</v>
-      </c>
-      <c r="AB22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.81029051452572631</v>
-      </c>
-      <c r="AC22" s="227">
-        <f t="shared" si="0"/>
+      <c r="D24" s="343" t="s">
+        <v>643</v>
+      </c>
+      <c r="E24" s="343" t="s">
+        <v>644</v>
+      </c>
+      <c r="F24" s="343">
         <v>1</v>
       </c>
-      <c r="AD22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.59990277102576572</v>
-      </c>
-      <c r="AE22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.59987929993964995</v>
-      </c>
-      <c r="AF22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.5998408910103421</v>
-      </c>
-      <c r="AG22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.59976662777129519</v>
-      </c>
-      <c r="AH22" s="227">
-        <f t="shared" si="0"/>
-        <v>0.5990675990675991</v>
-      </c>
-    </row>
-    <row r="28" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="N28" t="s">
-        <v>630</v>
-      </c>
-      <c r="O28" t="s">
-        <v>630</v>
-      </c>
-      <c r="P28" t="s">
-        <v>630</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>630</v>
-      </c>
-      <c r="R28" t="s">
-        <v>630</v>
-      </c>
-      <c r="S28" t="s">
-        <v>630</v>
-      </c>
-      <c r="T28" t="s">
-        <v>630</v>
-      </c>
-      <c r="U28" t="s">
-        <v>630</v>
-      </c>
-      <c r="V28" t="s">
-        <v>630</v>
-      </c>
-      <c r="W28" t="s">
-        <v>630</v>
-      </c>
-      <c r="X28" t="s">
-        <v>630</v>
-      </c>
-      <c r="Y28" t="s">
-        <v>630</v>
-      </c>
-      <c r="Z28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AA28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AC28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AD28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AE28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AF28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AG28" t="s">
-        <v>630</v>
-      </c>
-      <c r="AH28" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="29" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H29" t="s">
-        <v>631</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="G24" s="343">
+        <v>1</v>
+      </c>
+      <c r="H24" s="225"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C25" s="65" t="s">
+        <v>645</v>
+      </c>
+      <c r="D25" s="343" t="s">
+        <v>643</v>
+      </c>
+      <c r="E25" s="343" t="s">
+        <v>644</v>
+      </c>
+      <c r="F25" s="343">
+        <v>1.2</v>
+      </c>
+      <c r="G25" s="343">
+        <v>1.2</v>
+      </c>
+      <c r="H25" s="225"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="65" t="s">
+        <v>639</v>
+      </c>
+      <c r="D26" s="343" t="s">
+        <v>643</v>
+      </c>
+      <c r="E26" s="343" t="s">
+        <v>644</v>
+      </c>
+      <c r="F26" s="343"/>
+      <c r="G26" s="343"/>
+      <c r="H26" s="225"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C27" s="65" t="s">
+        <v>641</v>
+      </c>
+      <c r="D27" s="343" t="s">
+        <v>643</v>
+      </c>
+      <c r="E27" s="343" t="s">
+        <v>644</v>
+      </c>
+      <c r="F27" s="343"/>
+      <c r="G27" s="343"/>
+      <c r="H27" s="225"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C28" s="65"/>
+      <c r="D28" s="343"/>
+      <c r="E28" s="343"/>
+      <c r="F28" s="343"/>
+      <c r="G28" s="343"/>
+      <c r="H28" s="225"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C29" s="68"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="70"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="53" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="I53" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="Q53" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="X53" s="1" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="54" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="K54" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="W54" s="62" t="s">
+        <v>659</v>
+      </c>
+      <c r="X54">
+        <v>12</v>
+      </c>
+      <c r="Y54" s="347">
+        <f>X54/$X$56</f>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="55" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="J55" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="K55" s="345">
+        <f>'Chrome methodology'!F171</f>
+        <v>3.9494607908555515</v>
+      </c>
+      <c r="N55">
+        <f>'Chrome methodology'!P121</f>
+        <v>24</v>
+      </c>
+      <c r="W55" s="62" t="s">
+        <v>661</v>
+      </c>
+      <c r="X55">
+        <v>32</v>
+      </c>
+      <c r="Y55" s="347">
+        <f>X55/$X$56</f>
+        <v>0.72727272727272729</v>
+      </c>
+    </row>
+    <row r="56" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="J56" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="K56" s="345">
+        <f>'Chrome methodology'!F170</f>
+        <v>20.627230264875688</v>
+      </c>
+      <c r="N56">
+        <f>'Chrome methodology'!P122</f>
+        <v>28</v>
+      </c>
+      <c r="W56" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="J29" t="s">
-        <v>633</v>
-      </c>
-      <c r="K29" t="s">
-        <v>631</v>
-      </c>
-      <c r="L29" t="s">
-        <v>634</v>
-      </c>
-      <c r="M29" t="s">
-        <v>635</v>
-      </c>
-      <c r="N29">
-        <v>2019</v>
-      </c>
-      <c r="O29">
-        <v>2020</v>
-      </c>
-      <c r="P29">
-        <v>2021</v>
-      </c>
-      <c r="Q29">
-        <v>2022</v>
-      </c>
-      <c r="R29">
-        <v>2023</v>
-      </c>
-      <c r="S29">
-        <v>2024</v>
-      </c>
-      <c r="T29">
-        <v>2025</v>
-      </c>
-      <c r="U29">
-        <v>2026</v>
-      </c>
-      <c r="V29">
-        <v>2027</v>
-      </c>
-      <c r="W29">
-        <v>2028</v>
-      </c>
-      <c r="X29">
-        <v>2029</v>
-      </c>
-      <c r="Y29">
-        <v>2030</v>
-      </c>
-      <c r="Z29">
-        <v>2031</v>
-      </c>
-      <c r="AA29">
-        <v>2032</v>
-      </c>
-      <c r="AB29">
-        <v>2033</v>
-      </c>
-      <c r="AC29">
-        <v>2034</v>
-      </c>
-      <c r="AD29">
-        <v>2035</v>
-      </c>
-      <c r="AE29">
-        <v>2036</v>
-      </c>
-      <c r="AF29">
-        <v>2037</v>
-      </c>
-      <c r="AG29">
-        <v>2038</v>
-      </c>
-      <c r="AH29">
-        <v>2039</v>
-      </c>
-    </row>
-    <row r="30" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H30" t="s">
-        <v>636</v>
-      </c>
-      <c r="I30" t="s">
-        <v>637</v>
-      </c>
-      <c r="J30" t="s">
-        <v>638</v>
-      </c>
-      <c r="K30" t="s">
-        <v>636</v>
-      </c>
-      <c r="L30" t="s">
-        <v>605</v>
-      </c>
-      <c r="M30" t="s">
-        <v>639</v>
-      </c>
-      <c r="N30" s="323">
-        <v>3410</v>
-      </c>
-      <c r="O30" s="323">
-        <v>3097</v>
-      </c>
-      <c r="P30" s="323">
-        <v>3379</v>
-      </c>
-      <c r="Q30" s="323">
-        <v>3352</v>
-      </c>
-      <c r="R30" s="323">
-        <v>3356</v>
-      </c>
-      <c r="S30" s="323">
-        <v>3377</v>
-      </c>
-      <c r="T30" s="323">
-        <v>3402</v>
-      </c>
-      <c r="U30" s="323">
-        <v>3508</v>
-      </c>
-      <c r="V30" s="323">
-        <v>3601</v>
-      </c>
-      <c r="W30" s="323">
-        <v>3801</v>
-      </c>
-      <c r="X30" s="323">
-        <v>3953</v>
-      </c>
-      <c r="Y30" s="323">
-        <v>2434</v>
-      </c>
-      <c r="Z30" s="323">
-        <v>2194</v>
-      </c>
-      <c r="AA30" s="323">
-        <v>2197</v>
-      </c>
-      <c r="AB30" s="323">
-        <v>2315</v>
-      </c>
-      <c r="AC30" s="323">
-        <v>2457</v>
-      </c>
-      <c r="AD30" s="323">
-        <v>1234</v>
-      </c>
-      <c r="AE30">
-        <v>994</v>
-      </c>
-      <c r="AF30">
-        <v>754</v>
-      </c>
-      <c r="AG30">
-        <v>514</v>
-      </c>
-      <c r="AH30">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="31" spans="8:34" x14ac:dyDescent="0.2">
-      <c r="H31" t="s">
-        <v>214</v>
-      </c>
-      <c r="I31" t="s">
-        <v>637</v>
-      </c>
-      <c r="J31" t="s">
-        <v>638</v>
-      </c>
-      <c r="K31" t="s">
-        <v>214</v>
-      </c>
-      <c r="L31" t="s">
-        <v>605</v>
-      </c>
-      <c r="M31">
-        <v>0</v>
-      </c>
-      <c r="N31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="O31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="P31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="Q31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="R31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="S31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="T31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="U31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="V31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="W31" s="323">
-        <v>4857</v>
-      </c>
-      <c r="X31" s="323">
-        <v>4457</v>
-      </c>
-      <c r="Y31" s="323">
-        <v>4057</v>
-      </c>
-      <c r="Z31" s="323">
-        <v>3657</v>
-      </c>
-      <c r="AA31" s="323">
-        <v>3257</v>
-      </c>
-      <c r="AB31" s="323">
-        <v>2857</v>
-      </c>
-      <c r="AC31" s="323">
-        <v>2457</v>
-      </c>
-      <c r="AD31" s="323">
-        <v>2057</v>
-      </c>
-      <c r="AE31" s="323">
-        <v>1657</v>
-      </c>
-      <c r="AF31" s="323">
-        <v>1257</v>
-      </c>
-      <c r="AG31">
-        <v>857</v>
-      </c>
-      <c r="AH31">
-        <v>429</v>
+      <c r="X56" s="1">
+        <f>SUM(X54:X55)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="I58" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q58" s="62" t="s">
+        <v>657</v>
+      </c>
+      <c r="S58" s="62" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="59" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="K59" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="60" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="J60" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="K60" s="345">
+        <f>K55/N55</f>
+        <v>0.16456086628564798</v>
+      </c>
+      <c r="P60" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q60" s="346">
+        <v>0.8</v>
+      </c>
+      <c r="S60" s="345">
+        <f>Q60*K60</f>
+        <v>0.13164869302851839</v>
+      </c>
+    </row>
+    <row r="61" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="J61" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="K61" s="345">
+        <f>K56/N56</f>
+        <v>0.73668679517413171</v>
+      </c>
+      <c r="P61" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q61" s="346">
+        <v>0.9</v>
+      </c>
+      <c r="S61" s="345">
+        <f>Q61*K61</f>
+        <v>0.66301811565671853</v>
+      </c>
+    </row>
+    <row r="63" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="Q63" s="62" t="s">
+        <v>662</v>
+      </c>
+      <c r="S63" s="345">
+        <f>SUM(S60:S61)</f>
+        <v>0.79466680868523687</v>
+      </c>
+    </row>
+    <row r="64" spans="9:25" x14ac:dyDescent="0.2">
+      <c r="I64" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="R64" s="1"/>
+      <c r="S64" s="348">
+        <f>S63/Y54</f>
+        <v>2.9137782985125353</v>
+      </c>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="K65" s="1" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J66" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="K66">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J67" s="62" t="s">
+        <v>291</v>
+      </c>
+      <c r="K67">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="70" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I70" s="1" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="72" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J72" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="K72" s="345">
+        <f>K66*K60</f>
+        <v>0.51013868548550878</v>
+      </c>
+    </row>
+    <row r="73" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="K73" s="345">
+        <f>K67*K61</f>
+        <v>2.3573977445572214</v>
+      </c>
+    </row>
+    <row r="75" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J75" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="K75" s="345">
+        <f>SUM(K72:K73)</f>
+        <v>2.8675364300427302</v>
+      </c>
+    </row>
+    <row r="78" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I78" s="1" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="80" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="J80" s="345">
+        <f>K75</f>
+        <v>2.8675364300427302</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="81" spans="10:11" x14ac:dyDescent="0.2">
+      <c r="J81" s="345">
+        <f>S64</f>
+        <v>2.9137782985125353</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>666</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -27928,7 +27987,7 @@
       <pane xSplit="6" ySplit="7" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>